<commit_message>
XX files deleted and main merged
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/ae476_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{43B7B65F-1EE3-491F-BCC3-D8447C1EA81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A16BC37-EA45-4C43-8AE2-E9CDA1235004}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{43B7B65F-1EE3-491F-BCC3-D8447C1EA81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{853DE055-A90B-4B48-A47D-5EC04F59E1E4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -1813,46 +1813,46 @@
     <t>PK</t>
   </si>
   <si>
+    <t>1 Inv cost mean (EUR/Kw)</t>
+  </si>
+  <si>
+    <t>2 Inv Cost SD</t>
+  </si>
+  <si>
+    <t>3 O&amp;M mean (EUR/kW)</t>
+  </si>
+  <si>
+    <t>4 O&amp;M SD</t>
+  </si>
+  <si>
+    <t>7 Investment LR</t>
+  </si>
+  <si>
+    <t>10 Fuel cost  (EUR/kWh)</t>
+  </si>
+  <si>
+    <t>15 Emission factor</t>
+  </si>
+  <si>
+    <t>16 Payback time, mean</t>
+  </si>
+  <si>
+    <t>17 Payback time, SD</t>
+  </si>
+  <si>
+    <t>18 UD/FD</t>
+  </si>
+  <si>
+    <t>19 RES calc</t>
+  </si>
+  <si>
+    <t>20 Efficiency LR</t>
+  </si>
+  <si>
     <t>24 Aviation bunkers</t>
   </si>
   <si>
     <t>25 Marine bunkers</t>
-  </si>
-  <si>
-    <t>1 Inv cost mean (EUR/Kw)</t>
-  </si>
-  <si>
-    <t>2 Inv Cost SD</t>
-  </si>
-  <si>
-    <t>3 O&amp;M mean (EUR/kW)</t>
-  </si>
-  <si>
-    <t>4 O&amp;M SD</t>
-  </si>
-  <si>
-    <t>7 Investment LR</t>
-  </si>
-  <si>
-    <t>10 Fuel cost  (EUR/kWh)</t>
-  </si>
-  <si>
-    <t>15 Emission factor</t>
-  </si>
-  <si>
-    <t>16 Payback time, mean</t>
-  </si>
-  <si>
-    <t>17 Payback time, SD</t>
-  </si>
-  <si>
-    <t>18 UD/FD</t>
-  </si>
-  <si>
-    <t>19 RES calc</t>
-  </si>
-  <si>
-    <t>20 Efficiency LR</t>
   </si>
 </sst>
 </file>
@@ -2804,6 +2804,10 @@
 </inkml:ink>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5019,7 +5023,7 @@
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -5039,7 +5043,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5047,7 +5051,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5055,7 +5059,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -5063,7 +5067,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -5087,7 +5091,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -5111,7 +5115,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -5151,7 +5155,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -5159,7 +5163,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -5167,7 +5171,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -5175,7 +5179,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -5183,7 +5187,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -5191,7 +5195,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -7388,8 +7392,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7592,7 +7596,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>584</v>
+        <v>596</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -7600,7 +7604,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>585</v>
+        <v>597</v>
       </c>
       <c r="B26">
         <v>25</v>

</xml_diff>

<commit_message>
First attempt at adding new variables
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone_laptop_repos/FTT_StandAlone/Utilities/titles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{FE468311-42F7-4D79-8007-02B482EB8EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{444C9A47-71F8-4357-A355-AB6232F99739}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{FE468311-42F7-4D79-8007-02B482EB8EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1000857-6D4F-4AD6-BEB1-1C176EFF20C0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="9" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -35,10 +35,11 @@
     <sheet name="CTI" sheetId="18" r:id="rId20"/>
     <sheet name="TYTI" sheetId="25" r:id="rId21"/>
     <sheet name="VYTI" sheetId="19" r:id="rId22"/>
-    <sheet name="NA" sheetId="16" r:id="rId23"/>
-    <sheet name="MTI" sheetId="28" r:id="rId24"/>
-    <sheet name="ITTI" sheetId="32" r:id="rId25"/>
-    <sheet name="CTTI" sheetId="33" r:id="rId26"/>
+    <sheet name="battery_ages" sheetId="42" r:id="rId23"/>
+    <sheet name="NA" sheetId="16" r:id="rId24"/>
+    <sheet name="MTI" sheetId="28" r:id="rId25"/>
+    <sheet name="ITTI" sheetId="32" r:id="rId26"/>
+    <sheet name="CTTI" sheetId="33" r:id="rId27"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RTI!$A$1:$B$1</definedName>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="605">
   <si>
     <t>Full name</t>
   </si>
@@ -3125,7 +3126,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A6:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -4031,7 +4032,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -6820,7 +6821,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection sqref="A1:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7027,6 +7028,117 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA9CF4B-A8DC-429B-AA15-1A4FC4B58917}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F06019-7A65-4394-8ACA-0746C0360B24}">
   <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:B2"/>
@@ -7058,7 +7170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D88CEB-56EA-49AD-B799-67E4A3E7193E}">
   <sheetPr codeName="Sheet24"/>
   <dimension ref="A1:B11"/>
@@ -7166,7 +7278,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B303FD-D6D9-40A1-A2C1-8C222F1BD6AD}">
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:B14"/>
@@ -7298,7 +7410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF635E11-CE75-4103-893D-9384A23FD09B}">
   <sheetPr codeName="Sheet26"/>
   <dimension ref="A1:B16"/>
@@ -7450,7 +7562,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -9005,7 +9117,7 @@
   <dimension ref="A1:B995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B995"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
FTT-S: Classification Titles update 2_04062024
Added SMTI, SSTI, XPTI
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arpan.Golechha\Documents\GitHub\FTT_StandAlone\Utilities\titles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0D3F8D-0DFD-4E29-B28D-CB92B290B0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002BDAB9-62C5-40E6-B8D8-1D36B1A9599F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="9" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="12" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -41,6 +41,9 @@
     <sheet name="CTTI" sheetId="33" r:id="rId26"/>
     <sheet name="STTI" sheetId="35" r:id="rId27"/>
     <sheet name="C5TI" sheetId="36" r:id="rId28"/>
+    <sheet name="SMTI" sheetId="37" r:id="rId29"/>
+    <sheet name="SSTI" sheetId="38" r:id="rId30"/>
+    <sheet name="XTPI" sheetId="39" r:id="rId31"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RTI!$A$1:$B$1</definedName>
@@ -61,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="708">
   <si>
     <t>Full name</t>
   </si>
@@ -2098,6 +2101,93 @@
   </si>
   <si>
     <t>Biogas</t>
+  </si>
+  <si>
+    <t>Coke plant</t>
+  </si>
+  <si>
+    <t>Biocoke plant</t>
+  </si>
+  <si>
+    <t>Sinter plant</t>
+  </si>
+  <si>
+    <t>Biosinter plant</t>
+  </si>
+  <si>
+    <t>Pellet plant</t>
+  </si>
+  <si>
+    <t>Biopellet plant</t>
+  </si>
+  <si>
+    <t>Oxygen plant</t>
+  </si>
+  <si>
+    <t>Conv. BF</t>
+  </si>
+  <si>
+    <t>Conv. BF (BB)</t>
+  </si>
+  <si>
+    <t>BF TGR (CCS)</t>
+  </si>
+  <si>
+    <t>BF TGR (CCS, BB)</t>
+  </si>
+  <si>
+    <t>DR-gas</t>
+  </si>
+  <si>
+    <t>DR-gas (BB)</t>
+  </si>
+  <si>
+    <t>DR-coal</t>
+  </si>
+  <si>
+    <t>DR-coal (BB)</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>SR (BB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SR+ </t>
+  </si>
+  <si>
+    <t>SR+ (BB)</t>
+  </si>
+  <si>
+    <t>OHF</t>
+  </si>
+  <si>
+    <t>BOF</t>
+  </si>
+  <si>
+    <t>BOF (BB)</t>
+  </si>
+  <si>
+    <t>EAF</t>
+  </si>
+  <si>
+    <t>EAF (BB)</t>
+  </si>
+  <si>
+    <t>Final stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport </t>
+  </si>
+  <si>
+    <t>Machinery</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Products</t>
   </si>
 </sst>
 </file>
@@ -7669,9 +7759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31856602-FF94-44F9-856C-D5CCC04B2E09}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8265,6 +8353,222 @@
       </c>
       <c r="B43">
         <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EAFAFC-942E-4EAE-B407-B6352F555A88}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>659</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>660</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>661</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>662</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>663</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>664</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>665</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>666</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>667</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>668</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>669</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>670</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>671</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>672</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>673</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>674</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>675</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>676</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>677</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>678</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>637</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>639</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>650</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>641</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -8493,6 +8797,318 @@
       </c>
       <c r="B26">
         <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A2DBD6-286C-4F22-9C5E-A0D16FC294F4}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>679</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>680</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>681</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>682</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>683</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>684</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>685</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>686</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>687</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>688</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>689</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>690</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>691</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>692</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>693</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>694</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>695</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>696</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>697</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>636</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>698</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>699</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>700</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>701</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>702</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>633</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>635</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>636</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>703</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4CCE6EA-C83D-4184-8710-7BC586EE248C}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>704</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>705</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>706</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>707</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed a sheet in classification titles
Changed the sheet name from XTPI to XPTI
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arpan.Golechha\Documents\GitHub\FTT_StandAlone\Utilities\titles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002BDAB9-62C5-40E6-B8D8-1D36B1A9599F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E43579-3887-46D9-AFF0-479DCF956C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="12" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="12" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <sheet name="C5TI" sheetId="36" r:id="rId28"/>
     <sheet name="SMTI" sheetId="37" r:id="rId29"/>
     <sheet name="SSTI" sheetId="38" r:id="rId30"/>
-    <sheet name="XTPI" sheetId="39" r:id="rId31"/>
+    <sheet name="XPTI" sheetId="39" r:id="rId31"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RTI!$A$1:$B$1</definedName>
@@ -8808,7 +8808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A2DBD6-286C-4F22-9C5E-A0D16FC294F4}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9064,7 +9064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4CCE6EA-C83D-4184-8710-7BC586EE248C}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
new titles for shares
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CL852\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ib400\OneDrive - University of Exeter\Desktop\PhD\GitHub\FTT_StandAlone\Utilities\titles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21702BD4-B62F-4377-8B0D-0CBFF489688A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="19" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -43,7 +42,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RTI!$A$1:$B$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -59,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="624">
   <si>
     <t>Full name</t>
   </si>
@@ -1886,12 +1885,57 @@
   </si>
   <si>
     <t>20 Efficiency LR</t>
+  </si>
+  <si>
+    <t>shares_var</t>
+  </si>
+  <si>
+    <t>shares_roc_var</t>
+  </si>
+  <si>
+    <t>MEWS</t>
+  </si>
+  <si>
+    <t>MSRC</t>
+  </si>
+  <si>
+    <t>histend_var</t>
+  </si>
+  <si>
+    <t>MEWG</t>
+  </si>
+  <si>
+    <t>HEWS</t>
+  </si>
+  <si>
+    <t>TEWS</t>
+  </si>
+  <si>
+    <t>IWS1</t>
+  </si>
+  <si>
+    <t>IWS2</t>
+  </si>
+  <si>
+    <t>IWS3</t>
+  </si>
+  <si>
+    <t>IWS4</t>
+  </si>
+  <si>
+    <t>IWS5</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>HEWF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -3133,7 +3177,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC99D09-3987-4B67-BD77-8E3DA5ACCC31}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A6:H44"/>
   <sheetViews>
@@ -3425,24 +3469,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B12" location="'FUTI'!A1" display="'FUTI'!A1" xr:uid="{F5E71AA9-15E1-475E-BDF0-E991B3F7D4CF}"/>
-    <hyperlink ref="B13" location="'RTI'!A1" display="'RTI'!A1" xr:uid="{089679B9-2325-42BF-B831-ABC7311E7D20}"/>
-    <hyperlink ref="B14" location="'ERTI'!A1" display="'ERTI'!A1" xr:uid="{F2A8C563-6BE6-4594-AFCC-E8CECE4FC503}"/>
-    <hyperlink ref="B15" location="'JTI'!A1" display="'JTI'!A1" xr:uid="{EBE5020C-E897-43B9-B004-956665EAE3AB}"/>
-    <hyperlink ref="B16" location="'VTTI'!A1" display="'VTTI'!A1" xr:uid="{048D7160-D43C-4BB3-A7E9-3A02D15084B9}"/>
-    <hyperlink ref="B17" location="'CSCTI'!A1" display="'CSCTI'!A1" xr:uid="{ADA5EC3F-C320-4E41-BC30-97DEF8236625}"/>
-    <hyperlink ref="B18" location="'YTI'!A1" display="'YTI'!A1" xr:uid="{162CAC2B-8784-42E0-B83C-AFF47AD201BE}"/>
-    <hyperlink ref="B19" location="'C3TI'!A1" display="'C3TI'!A1" xr:uid="{B478498A-08C3-4FEA-BFC7-AE385A0BB28F}"/>
-    <hyperlink ref="B20" location="'T2TI'!A1" display="'T2TI'!A1" xr:uid="{08E2FE1F-2A29-417E-9E24-2E204649473A}"/>
-    <hyperlink ref="B21" location="'C2TI'!A1" display="'C2TI'!A1" xr:uid="{B115F602-7A6B-4B0C-B9B0-BD6C28F1A627}"/>
-    <hyperlink ref="B22" location="'LBTI'!A1" display="'LBTI'!A1" xr:uid="{BD93AE32-9C29-4BF9-A1F2-18849BBC088D}"/>
-    <hyperlink ref="B23" location="'HTTI'!A1" display="'HTTI'!A1" xr:uid="{39557502-B8A8-4997-B43B-6C276B737E77}"/>
-    <hyperlink ref="B24" location="'C4TI'!A1" display="'C4TI'!A1" xr:uid="{2526562A-21A7-4293-82A5-ADE84400329C}"/>
-    <hyperlink ref="B25" location="'DPTI'!A1" display="'DPTI'!A1" xr:uid="{D22F6BAD-1F73-401A-A871-AC8143689C5E}"/>
-    <hyperlink ref="B26" location="'CTI'!A1" display="'CTI'!A1" xr:uid="{EAF9BE45-2806-45E6-B69F-430B787670CB}"/>
-    <hyperlink ref="B27" location="'TYTI'!A1" display="'TYTI'!A1" xr:uid="{1CF8CB4B-A910-4C10-8BE2-9A358083D648}"/>
-    <hyperlink ref="B28" location="'VYTI'!A1" display="'VYTI'!A1" xr:uid="{1A4F4F63-2282-47C2-834C-AA7A0B4FB0C8}"/>
-    <hyperlink ref="B29" location="'NA'!A1" display="'NA'!A1" xr:uid="{A94005FD-BDDA-4B22-811F-DC97572FE157}"/>
+    <hyperlink ref="B12" location="'FUTI'!A1" display="'FUTI'!A1"/>
+    <hyperlink ref="B13" location="'RTI'!A1" display="'RTI'!A1"/>
+    <hyperlink ref="B14" location="'ERTI'!A1" display="'ERTI'!A1"/>
+    <hyperlink ref="B15" location="'JTI'!A1" display="'JTI'!A1"/>
+    <hyperlink ref="B16" location="'VTTI'!A1" display="'VTTI'!A1"/>
+    <hyperlink ref="B17" location="'CSCTI'!A1" display="'CSCTI'!A1"/>
+    <hyperlink ref="B18" location="'YTI'!A1" display="'YTI'!A1"/>
+    <hyperlink ref="B19" location="'C3TI'!A1" display="'C3TI'!A1"/>
+    <hyperlink ref="B20" location="'T2TI'!A1" display="'T2TI'!A1"/>
+    <hyperlink ref="B21" location="'C2TI'!A1" display="'C2TI'!A1"/>
+    <hyperlink ref="B22" location="'LBTI'!A1" display="'LBTI'!A1"/>
+    <hyperlink ref="B23" location="'HTTI'!A1" display="'HTTI'!A1"/>
+    <hyperlink ref="B24" location="'C4TI'!A1" display="'C4TI'!A1"/>
+    <hyperlink ref="B25" location="'DPTI'!A1" display="'DPTI'!A1"/>
+    <hyperlink ref="B26" location="'CTI'!A1" display="'CTI'!A1"/>
+    <hyperlink ref="B27" location="'TYTI'!A1" display="'TYTI'!A1"/>
+    <hyperlink ref="B28" location="'VYTI'!A1" display="'VYTI'!A1"/>
+    <hyperlink ref="B29" location="'NA'!A1" display="'NA'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3451,7 +3495,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C18603C-7A3A-4CC2-AD59-D8B2B46E22BF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:B71"/>
   <sheetViews>
@@ -4039,11 +4083,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18DFFF2-8EA6-44E6-8D28-E9465D14B196}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -4244,11 +4288,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C84BF1-D202-40D0-9C0C-F82CFDCF6C25}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -4463,7 +4507,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C01FE79-1B64-410C-BFB3-7EE7C4F3E8BE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:B22"/>
   <sheetViews>
@@ -4658,7 +4702,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E76AE8C-AA73-4A64-A81D-4A07EE993B70}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -4845,7 +4889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92305D15-A7CF-4383-AF5B-98B7C49C2AEB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -4885,7 +4929,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C61870-7715-450E-B5AC-EEF1B774E191}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -4957,7 +5001,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34EEFDEC-9661-454F-B5C9-8D81DE9B0DC3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -5089,7 +5133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37811D6B-EDD0-4FFA-9045-B8E106F2C185}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -5277,7 +5321,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25819D4-BF1F-4D53-BC0A-C08E72C9848D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -5497,21 +5541,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AE06A4-CDB3-4DA5-AA93-26CDCBA71A9A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D1" sqref="D1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5521,8 +5569,17 @@
       <c r="C1" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>609</v>
+      </c>
+      <c r="E1" t="s">
+        <v>610</v>
+      </c>
+      <c r="F1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>543</v>
       </c>
@@ -5532,8 +5589,17 @@
       <c r="C2" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>611</v>
+      </c>
+      <c r="E2" t="s">
+        <v>612</v>
+      </c>
+      <c r="F2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>545</v>
       </c>
@@ -5543,8 +5609,17 @@
       <c r="C3" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>615</v>
+      </c>
+      <c r="E3" t="s">
+        <v>622</v>
+      </c>
+      <c r="F3" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>565</v>
       </c>
@@ -5554,8 +5629,17 @@
       <c r="C4" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>616</v>
+      </c>
+      <c r="E4" t="s">
+        <v>622</v>
+      </c>
+      <c r="F4" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>568</v>
       </c>
@@ -5565,8 +5649,17 @@
       <c r="C5" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>622</v>
+      </c>
+      <c r="E5" t="s">
+        <v>622</v>
+      </c>
+      <c r="F5" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>544</v>
       </c>
@@ -5576,8 +5669,17 @@
       <c r="C6" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>617</v>
+      </c>
+      <c r="E6" t="s">
+        <v>622</v>
+      </c>
+      <c r="F6" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>557</v>
       </c>
@@ -5587,8 +5689,17 @@
       <c r="C7" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>618</v>
+      </c>
+      <c r="E7" t="s">
+        <v>622</v>
+      </c>
+      <c r="F7" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>558</v>
       </c>
@@ -5598,8 +5709,17 @@
       <c r="C8" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>619</v>
+      </c>
+      <c r="E8" t="s">
+        <v>622</v>
+      </c>
+      <c r="F8" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>559</v>
       </c>
@@ -5609,8 +5729,17 @@
       <c r="C9" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>620</v>
+      </c>
+      <c r="E9" t="s">
+        <v>622</v>
+      </c>
+      <c r="F9" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>564</v>
       </c>
@@ -5620,14 +5749,24 @@
       <c r="C10" t="s">
         <v>556</v>
       </c>
+      <c r="D10" t="s">
+        <v>621</v>
+      </c>
+      <c r="E10" t="s">
+        <v>622</v>
+      </c>
+      <c r="F10" t="s">
+        <v>622</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E505B4BB-C670-480F-A1C1-143C2BAC14E5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:B44"/>
   <sheetViews>
@@ -5999,7 +6138,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F24619-4495-45A3-B0D1-A626CB4F5E9C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:B101"/>
   <sheetViews>
@@ -6827,7 +6966,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971A201D-DA84-43FC-9703-0E5C242ECDDA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:B24"/>
   <sheetViews>
@@ -7039,11 +7178,11 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F06019-7A65-4394-8ACA-0746C0360B24}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -7071,7 +7210,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D88CEB-56EA-49AD-B799-67E4A3E7193E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet24"/>
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -7179,7 +7318,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B303FD-D6D9-40A1-A2C1-8C222F1BD6AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -7311,7 +7450,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF635E11-CE75-4103-893D-9384A23FD09B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet26"/>
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -7458,7 +7597,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D24AC0-AB7E-4652-ACEE-CA80D4873B0D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B26"/>
   <sheetViews>
@@ -7686,7 +7825,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B2B9FEF-82E7-479E-BB9A-C13F50F190CD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B72"/>
   <sheetViews>
@@ -8277,8 +8416,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1" xr:uid="{3B2B9FEF-82E7-479E-BB9A-C13F50F190CD}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B33">
+  <autoFilter ref="A1:B1">
+    <sortState ref="A2:B33">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
@@ -8287,7 +8426,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B1B8E3-9CDC-45F6-8F23-461491FFAE16}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -8426,7 +8565,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584A6227-8B0F-47D1-9E3E-191843EE9974}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -8550,7 +8689,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7D7645-A5D2-494E-B37B-AD0167F8F0B3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:B32"/>
   <sheetViews>
@@ -8825,7 +8964,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56AA3A07-21BA-4ACD-867A-E4F0D5D67CE0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -9012,7 +9151,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97775261-153B-49B0-AC61-D3694494D674}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:B995"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add Steel to front end
Note, output in SEWS, SJEF is 0. Also fixes a minor spelling error in VariableListing that was preventing update_manager_metadata.py from running.
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="106_{D04AC8C1-929F-4285-8B5B-9F972A603C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="106_{D04AC8C1-929F-4285-8B5B-9F972A603C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{451CE33C-06D3-4D2C-B78A-F116CC9F48B6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="21" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="711">
   <si>
     <t>Full name</t>
   </si>
@@ -2189,6 +2189,15 @@
   </si>
   <si>
     <t>Products</t>
+  </si>
+  <si>
+    <t>steel</t>
+  </si>
+  <si>
+    <t>FTT-S</t>
+  </si>
+  <si>
+    <t>SGAM</t>
   </si>
 </sst>
 </file>
@@ -5800,10 +5809,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AE06A4-CDB3-4DA5-AA93-26CDCBA71A9A}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5920,6 +5929,17 @@
       </c>
       <c r="C10" t="s">
         <v>556</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>708</v>
+      </c>
+      <c r="B11" t="s">
+        <v>709</v>
+      </c>
+      <c r="C11" t="s">
+        <v>710</v>
       </c>
     </row>
   </sheetData>
@@ -7760,7 +7780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31856602-FF94-44F9-856C-D5CCC04B2E09}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0"/>
+    <sheetView topLeftCell="A17" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
fix initial errors merge
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{21702BD4-B62F-4377-8B0D-0CBFF489688A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57B95B7D-65E5-4591-954B-19090C950E1A}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{21702BD4-B62F-4377-8B0D-0CBFF489688A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1FE560D-DCB5-4C75-AFAA-8E77DEAF997E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" firstSheet="11" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -507,9 +507,6 @@
     <t>20 Baseload (0 or 1)</t>
   </si>
   <si>
-    <t>21 Empty</t>
-  </si>
-  <si>
     <t>1 Baseload</t>
   </si>
   <si>
@@ -1912,6 +1909,9 @@
   </si>
   <si>
     <t>Starting degradation</t>
+  </si>
+  <si>
+    <t>21 Gamma ($/MWh)</t>
   </si>
 </sst>
 </file>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3216,137 +3216,137 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>11</v>
@@ -3356,7 +3356,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>8</v>
@@ -3367,7 +3367,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>9</v>
@@ -3378,7 +3378,7 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>10</v>
@@ -3392,7 +3392,7 @@
         <v>12</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -3400,10 +3400,10 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>609</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>610</v>
       </c>
       <c r="H30" s="3"/>
     </row>
@@ -4198,7 +4198,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -4230,7 +4230,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -4238,7 +4238,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -4246,7 +4246,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -4254,7 +4254,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -4262,7 +4262,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -4298,7 +4298,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4306,7 +4306,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -4314,7 +4314,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -4322,7 +4322,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -4330,7 +4330,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -4338,7 +4338,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -4346,7 +4346,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -4354,7 +4354,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -4362,7 +4362,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -4370,7 +4370,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -4378,7 +4378,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -4386,7 +4386,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -4394,7 +4394,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -4402,7 +4402,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -4410,7 +4410,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -4418,7 +4418,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -4426,7 +4426,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -4434,7 +4434,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -4442,7 +4442,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -4450,7 +4450,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -4458,7 +4458,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -4466,7 +4466,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -4474,7 +4474,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -4482,7 +4482,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -4498,8 +4498,8 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4677,7 +4677,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>148</v>
+        <v>616</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -4712,7 +4712,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4720,7 +4720,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -4736,7 +4736,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -4752,7 +4752,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -4768,7 +4768,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -4776,7 +4776,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -4784,7 +4784,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -4792,7 +4792,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -4800,7 +4800,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -4808,7 +4808,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -4816,7 +4816,7 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -4824,7 +4824,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -4832,7 +4832,7 @@
     </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -4840,7 +4840,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -4848,7 +4848,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -4856,7 +4856,7 @@
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -4864,7 +4864,7 @@
     </row>
     <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -4896,7 +4896,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4904,7 +4904,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -4936,7 +4936,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4944,7 +4944,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -4952,7 +4952,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -4960,7 +4960,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -4968,7 +4968,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -4976,7 +4976,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -5012,7 +5012,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5020,7 +5020,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5028,7 +5028,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -5036,7 +5036,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -5044,7 +5044,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -5052,7 +5052,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -5060,7 +5060,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -5068,7 +5068,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -5076,7 +5076,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -5084,7 +5084,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -5092,7 +5092,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -5100,7 +5100,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -5108,7 +5108,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -5144,7 +5144,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5152,7 +5152,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5160,7 +5160,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -5168,7 +5168,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -5176,7 +5176,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -5184,7 +5184,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -5192,7 +5192,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -5200,7 +5200,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -5208,7 +5208,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -5216,7 +5216,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -5224,7 +5224,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -5232,7 +5232,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -5240,7 +5240,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -5248,7 +5248,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -5256,7 +5256,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -5264,7 +5264,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -5272,7 +5272,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -5280,7 +5280,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -5288,7 +5288,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -5296,7 +5296,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -5332,7 +5332,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5340,7 +5340,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5348,7 +5348,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -5356,7 +5356,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -5364,7 +5364,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -5372,7 +5372,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -5380,7 +5380,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -5388,7 +5388,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -5396,7 +5396,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -5404,7 +5404,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -5412,7 +5412,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -5420,7 +5420,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -5428,7 +5428,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -5436,7 +5436,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -5444,7 +5444,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -5452,7 +5452,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -5460,7 +5460,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -5468,7 +5468,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -5476,7 +5476,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -5484,7 +5484,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -5492,7 +5492,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -5500,7 +5500,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -5508,7 +5508,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -5516,7 +5516,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -5550,106 +5550,106 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>564</v>
+      </c>
+      <c r="B4" t="s">
+        <v>566</v>
+      </c>
+      <c r="C4" t="s">
         <v>565</v>
-      </c>
-      <c r="B4" t="s">
-        <v>567</v>
-      </c>
-      <c r="C4" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>567</v>
+      </c>
+      <c r="B5" t="s">
         <v>568</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>569</v>
-      </c>
-      <c r="C5" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B6" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C6" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B7" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C8" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B9" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C9" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B10" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -5682,7 +5682,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5690,7 +5690,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5698,7 +5698,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -5706,7 +5706,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -5714,7 +5714,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -5722,7 +5722,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -5730,7 +5730,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -5738,7 +5738,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -5746,7 +5746,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -5754,7 +5754,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -5762,7 +5762,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -5770,7 +5770,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -5778,7 +5778,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -5786,7 +5786,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -5794,7 +5794,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -5802,7 +5802,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -5810,7 +5810,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -5818,7 +5818,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -5826,7 +5826,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -5834,7 +5834,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -5842,7 +5842,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -5850,7 +5850,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -5858,7 +5858,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -5866,7 +5866,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -5874,7 +5874,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -5882,7 +5882,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -5890,7 +5890,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -5898,7 +5898,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -5906,7 +5906,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -5914,7 +5914,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -5922,7 +5922,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -5930,7 +5930,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -5938,7 +5938,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -5946,7 +5946,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -5954,7 +5954,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -5962,7 +5962,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -5970,7 +5970,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -5978,7 +5978,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -5986,7 +5986,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -5994,7 +5994,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -6002,7 +6002,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -6010,7 +6010,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -6018,7 +6018,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B44">
         <v>43</v>
@@ -7235,7 +7235,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7243,7 +7243,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7251,7 +7251,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7259,7 +7259,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -7267,7 +7267,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -7275,7 +7275,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -7283,7 +7283,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -7291,7 +7291,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -7299,7 +7299,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -7307,7 +7307,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -7343,7 +7343,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7351,7 +7351,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7359,7 +7359,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7367,7 +7367,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -7375,7 +7375,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -7383,7 +7383,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -7391,7 +7391,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -7399,7 +7399,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -7407,7 +7407,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -7415,7 +7415,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -7423,7 +7423,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -7431,7 +7431,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -7439,7 +7439,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -7474,7 +7474,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7482,7 +7482,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7490,7 +7490,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7498,7 +7498,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -7506,7 +7506,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -7514,7 +7514,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -7522,7 +7522,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -7530,7 +7530,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -7538,7 +7538,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -7546,7 +7546,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -7554,7 +7554,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -7562,7 +7562,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -7570,7 +7570,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -7578,7 +7578,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -7586,7 +7586,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -7601,7 +7601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC78C90-B6A7-480E-A2B9-E4BD1826822A}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -7617,7 +7617,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7625,7 +7625,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7633,7 +7633,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7641,7 +7641,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -7649,7 +7649,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -7657,7 +7657,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -7665,7 +7665,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -7673,7 +7673,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -7681,7 +7681,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -7689,7 +7689,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -7697,7 +7697,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -7705,7 +7705,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -7713,7 +7713,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -7721,7 +7721,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -7757,7 +7757,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7765,7 +7765,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7773,7 +7773,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7781,7 +7781,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -7789,7 +7789,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -7797,7 +7797,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -7805,7 +7805,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -7813,7 +7813,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -7821,7 +7821,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -7829,7 +7829,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -7837,7 +7837,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -7845,7 +7845,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -7853,7 +7853,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -7861,7 +7861,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -7869,7 +7869,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -7877,7 +7877,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -7885,7 +7885,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -7893,7 +7893,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -7901,7 +7901,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -7909,7 +7909,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -7917,7 +7917,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -7925,7 +7925,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -7933,7 +7933,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -7941,7 +7941,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -7949,7 +7949,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -7985,119 +7985,119 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -8105,151 +8105,151 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B27" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B31" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B32" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B33" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -8257,298 +8257,298 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B37" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B38" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B39" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B40" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B41" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B42" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B43" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B44" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B45" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B46" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B47" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B48" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B50" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B51" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B52" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B53" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B54" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B55" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B56" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B57" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B58" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B59" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B60" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B61" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B62" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B63" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B64" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B65" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B66" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B67" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B68" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B69" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B70" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B71" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>570</v>
+      </c>
+      <c r="B72" t="s">
         <v>571</v>
-      </c>
-      <c r="B72" t="s">
-        <v>572</v>
       </c>
     </row>
   </sheetData>
@@ -8585,7 +8585,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -8593,7 +8593,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -8601,7 +8601,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -8609,7 +8609,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -8617,7 +8617,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -8625,7 +8625,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -8633,7 +8633,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -8641,7 +8641,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -8649,7 +8649,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -8657,7 +8657,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -8665,7 +8665,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -8673,7 +8673,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -8681,7 +8681,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -8689,7 +8689,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -8856,7 +8856,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -8944,7 +8944,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -8952,7 +8952,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -8960,7 +8960,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -9016,7 +9016,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -9024,7 +9024,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -9032,7 +9032,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -9040,7 +9040,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -9048,7 +9048,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -9056,7 +9056,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -9064,7 +9064,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -9072,7 +9072,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -9080,7 +9080,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -9088,7 +9088,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -9123,7 +9123,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -9131,7 +9131,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -9139,7 +9139,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -9147,7 +9147,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -9155,7 +9155,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -9163,7 +9163,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -9171,7 +9171,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -9179,7 +9179,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -9187,7 +9187,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -9195,7 +9195,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -9203,7 +9203,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -9211,7 +9211,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -9219,7 +9219,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -9227,7 +9227,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -9235,7 +9235,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -9243,7 +9243,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -9251,7 +9251,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -9259,7 +9259,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -9267,7 +9267,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -9275,7 +9275,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -9310,34 +9310,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add noit and models_w_batteries to classification
And made a start with the V2G implementation.
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{21702BD4-B62F-4377-8B0D-0CBFF489688A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1FE560D-DCB5-4C75-AFAA-8E77DEAF997E}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{21702BD4-B62F-4377-8B0D-0CBFF489688A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31206F83-8E32-4F9A-8AE2-3247EF050D69}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" firstSheet="13" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -41,6 +41,8 @@
     <sheet name="ITTI" sheetId="32" r:id="rId26"/>
     <sheet name="CTTI" sheetId="33" r:id="rId27"/>
     <sheet name="SCA" sheetId="37" r:id="rId28"/>
+    <sheet name="noit" sheetId="40" r:id="rId29"/>
+    <sheet name="models_w_batteries" sheetId="41" r:id="rId30"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RTI!$A$1:$B$1</definedName>
@@ -61,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="622">
   <si>
     <t>Full name</t>
   </si>
@@ -1912,6 +1914,21 @@
   </si>
   <si>
     <t>21 Gamma ($/MWh)</t>
+  </si>
+  <si>
+    <t>V2G available fraction</t>
+  </si>
+  <si>
+    <t>V2G participation rate</t>
+  </si>
+  <si>
+    <t>FTT:P</t>
+  </si>
+  <si>
+    <t>FTT:Tr</t>
+  </si>
+  <si>
+    <t>FTT:Fr</t>
   </si>
 </sst>
 </file>
@@ -2863,6 +2880,10 @@
 </inkml:ink>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -4498,7 +4519,7 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -6862,7 +6883,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7602,7 +7623,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7657,7 +7678,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -7665,7 +7686,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -7725,6 +7746,61 @@
       </c>
       <c r="B15">
         <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0A2F22-28FA-49F7-8288-13E6FAEB1B52}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -7953,6 +8029,53 @@
       </c>
       <c r="B26">
         <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB217666-0838-4EF6-98D7-EB802105615C}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>619</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>620</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>621</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -9292,7 +9415,7 @@
   <dimension ref="A1:B995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B995"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implement simple battery LBD
First draft.

Note: there is little effect of anything on FTT:Fr. Is it possible that there is an error in lcof?
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{21702BD4-B62F-4377-8B0D-0CBFF489688A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31206F83-8E32-4F9A-8AE2-3247EF050D69}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{21702BD4-B62F-4377-8B0D-0CBFF489688A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5179899B-2D04-4A44-B53D-A5F5D2AF7B58}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" firstSheet="13" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" firstSheet="13" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="624">
   <si>
     <t>Full name</t>
   </si>
@@ -1929,6 +1929,12 @@
   </si>
   <si>
     <t>FTT:Fr</t>
+  </si>
+  <si>
+    <t>21 Battery capacity (kWh)</t>
+  </si>
+  <si>
+    <t>Battery learning exponent</t>
   </si>
 </sst>
 </file>
@@ -2880,10 +2886,6 @@
 </inkml:ink>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -4712,10 +4714,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E76AE8C-AA73-4A64-A81D-4A07EE993B70}">
   <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4889,6 +4891,14 @@
       </c>
       <c r="B21">
         <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>622</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -7622,8 +7632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC78C90-B6A7-480E-A2B9-E4BD1826822A}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7694,7 +7704,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>614</v>
+        <v>623</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -8040,7 +8050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB217666-0838-4EF6-98D7-EB802105615C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix couple of bugs
Bugs after cherry pick in classification and lcoe
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4E51A727-BBFB-DF4A-BD87-EDD223C8F174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDC55C90-66F2-43E4-B8DC-E4B365164D32}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{4E51A727-BBFB-DF4A-BD87-EDD223C8F174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCB9B803-9259-4336-A8BB-9B0F912AA14D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="607">
   <si>
     <t>Full name</t>
   </si>
@@ -811,42 +811,12 @@
     <t>4 Coal + CCS</t>
   </si>
   <si>
-    <t>5 IGCC</t>
-  </si>
-  <si>
-    <t>6 IGCC + CCS</t>
-  </si>
-  <si>
     <t>7 CCGT</t>
   </si>
   <si>
     <t>8 CCGT + CCS</t>
   </si>
   <si>
-    <t>9 Solid Biomass</t>
-  </si>
-  <si>
-    <t>10 S Biomass CCS</t>
-  </si>
-  <si>
-    <t>11 BIGCC</t>
-  </si>
-  <si>
-    <t>12 BIGCC + CCS</t>
-  </si>
-  <si>
-    <t>13 Biogas</t>
-  </si>
-  <si>
-    <t>14 Biogas + CCS</t>
-  </si>
-  <si>
-    <t>15 Tidal</t>
-  </si>
-  <si>
-    <t>16 Large Hydro</t>
-  </si>
-  <si>
     <t>17 Onshore</t>
   </si>
   <si>
@@ -859,18 +829,6 @@
     <t>20 CSP</t>
   </si>
   <si>
-    <t>21 Geothermal</t>
-  </si>
-  <si>
-    <t>22 Wave</t>
-  </si>
-  <si>
-    <t>23 Fuel Cells</t>
-  </si>
-  <si>
-    <t>24 CHP</t>
-  </si>
-  <si>
     <t>4 Gas</t>
   </si>
   <si>
@@ -1886,6 +1844,42 @@
   </si>
   <si>
     <t>21 Gamma ($/MWh)</t>
+  </si>
+  <si>
+    <t>5 Waste</t>
+  </si>
+  <si>
+    <t>6 Waste + CCS</t>
+  </si>
+  <si>
+    <t>9 OCGT</t>
+  </si>
+  <si>
+    <t>10 OCGT + CCS</t>
+  </si>
+  <si>
+    <t>11 Biomass</t>
+  </si>
+  <si>
+    <t>12 Biomass + CCS</t>
+  </si>
+  <si>
+    <t>13 Large Hydro</t>
+  </si>
+  <si>
+    <t>14 Pumped Hydro</t>
+  </si>
+  <si>
+    <t>15 Geothermal</t>
+  </si>
+  <si>
+    <t>16 Marine</t>
+  </si>
+  <si>
+    <t>21 Fuel cells / Turbine</t>
+  </si>
+  <si>
+    <t>22 Lithium-ion</t>
   </si>
 </sst>
 </file>
@@ -3166,7 +3160,7 @@
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16" t="s">
-        <v>477</v>
+        <v>463</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3190,137 +3184,137 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="3" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="3" t="s">
-        <v>448</v>
+        <v>434</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="3" t="s">
-        <v>449</v>
+        <v>435</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>467</v>
+        <v>453</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="3" t="s">
-        <v>450</v>
+        <v>436</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="3" t="s">
-        <v>451</v>
+        <v>437</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>468</v>
+        <v>454</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="3" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="3" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>470</v>
+        <v>456</v>
       </c>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="3" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>471</v>
+        <v>457</v>
       </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="3" t="s">
-        <v>455</v>
+        <v>441</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="3" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="3" t="s">
-        <v>457</v>
+        <v>443</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="3" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>475</v>
+        <v>461</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="3" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>11</v>
@@ -3330,7 +3324,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="3" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>8</v>
@@ -3341,7 +3335,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="3" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>9</v>
@@ -3352,7 +3346,7 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="3" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>10</v>
@@ -3366,7 +3360,7 @@
         <v>12</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -4167,7 +4161,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>592</v>
+        <v>578</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -4199,7 +4193,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>577</v>
+        <v>563</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -4207,7 +4201,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>576</v>
+        <v>562</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -4215,7 +4209,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>575</v>
+        <v>561</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -4223,7 +4217,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>574</v>
+        <v>560</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -4231,7 +4225,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>573</v>
+        <v>559</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -4246,10 +4240,10 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C84BF1-D202-40D0-9C0C-F82CFDCF6C25}">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4299,7 +4293,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>250</v>
+        <v>595</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -4307,7 +4301,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>251</v>
+        <v>596</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -4315,7 +4309,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -4323,7 +4317,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -4331,7 +4325,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>254</v>
+        <v>597</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -4339,7 +4333,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>255</v>
+        <v>598</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -4347,7 +4341,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>256</v>
+        <v>599</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -4355,7 +4349,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>257</v>
+        <v>600</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -4363,7 +4357,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>258</v>
+        <v>601</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -4371,7 +4365,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>259</v>
+        <v>602</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -4379,7 +4373,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>260</v>
+        <v>603</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -4387,7 +4381,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>261</v>
+        <v>604</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -4395,7 +4389,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -4403,7 +4397,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -4411,7 +4405,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -4419,7 +4413,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -4427,7 +4421,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>266</v>
+        <v>605</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -4435,26 +4429,10 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>267</v>
+        <v>606</v>
       </c>
       <c r="B23">
         <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>268</v>
-      </c>
-      <c r="B24">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>269</v>
-      </c>
-      <c r="B25">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -4467,7 +4445,7 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -4646,7 +4624,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>608</v>
+        <v>594</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -4681,7 +4659,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>508</v>
+        <v>494</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4689,7 +4667,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -4705,7 +4683,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -4721,7 +4699,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>519</v>
+        <v>505</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -4737,7 +4715,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -4745,7 +4723,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -4753,7 +4731,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>516</v>
+        <v>502</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -4761,7 +4739,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -4769,7 +4747,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>514</v>
+        <v>500</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -4777,7 +4755,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>605</v>
+        <v>591</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -4785,7 +4763,7 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -4793,7 +4771,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -4801,7 +4779,7 @@
     </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>572</v>
+        <v>558</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -4809,7 +4787,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>511</v>
+        <v>497</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -4817,7 +4795,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -4825,7 +4803,7 @@
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -4833,7 +4811,7 @@
     </row>
     <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>520</v>
+        <v>506</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -4865,7 +4843,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4873,7 +4851,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5113,7 +5091,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5121,7 +5099,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>594</v>
+        <v>580</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5129,7 +5107,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>595</v>
+        <v>581</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -5137,7 +5115,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>596</v>
+        <v>582</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -5161,7 +5139,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>597</v>
+        <v>583</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -5185,7 +5163,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>598</v>
+        <v>584</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -5225,7 +5203,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>599</v>
+        <v>585</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -5233,7 +5211,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>600</v>
+        <v>586</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -5241,7 +5219,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>601</v>
+        <v>587</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -5249,7 +5227,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>602</v>
+        <v>588</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -5257,7 +5235,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>603</v>
+        <v>589</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -5265,7 +5243,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>604</v>
+        <v>590</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -5519,106 +5497,106 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>541</v>
+        <v>527</v>
       </c>
       <c r="B2" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
       <c r="C2" t="s">
-        <v>548</v>
+        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>543</v>
+        <v>529</v>
       </c>
       <c r="B3" t="s">
-        <v>545</v>
+        <v>531</v>
       </c>
       <c r="C3" t="s">
-        <v>549</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>561</v>
+        <v>547</v>
       </c>
       <c r="B4" t="s">
-        <v>563</v>
+        <v>549</v>
       </c>
       <c r="C4" t="s">
-        <v>562</v>
+        <v>548</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>564</v>
+        <v>550</v>
       </c>
       <c r="B5" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
       <c r="C5" t="s">
-        <v>566</v>
+        <v>552</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>542</v>
+        <v>528</v>
       </c>
       <c r="B6" t="s">
-        <v>546</v>
+        <v>532</v>
       </c>
       <c r="C6" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="B7" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="C7" t="s">
-        <v>551</v>
+        <v>537</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>556</v>
+        <v>542</v>
       </c>
       <c r="B8" t="s">
-        <v>559</v>
+        <v>545</v>
       </c>
       <c r="C8" t="s">
-        <v>552</v>
+        <v>538</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>557</v>
+        <v>543</v>
       </c>
       <c r="B9" t="s">
-        <v>560</v>
+        <v>546</v>
       </c>
       <c r="C9" t="s">
-        <v>553</v>
+        <v>539</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>606</v>
+        <v>592</v>
       </c>
       <c r="B10" t="s">
-        <v>607</v>
+        <v>593</v>
       </c>
       <c r="C10" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
     </row>
   </sheetData>
@@ -7095,7 +7073,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7103,7 +7081,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7111,7 +7089,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7119,7 +7097,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>481</v>
+        <v>467</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -7127,7 +7105,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -7135,7 +7113,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -7143,7 +7121,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -7151,7 +7129,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -7159,7 +7137,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -7167,7 +7145,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>487</v>
+        <v>473</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -7203,7 +7181,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>524</v>
+        <v>510</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7211,7 +7189,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7219,7 +7197,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7227,7 +7205,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>527</v>
+        <v>513</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -7235,7 +7213,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -7243,7 +7221,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -7251,7 +7229,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -7259,7 +7237,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>531</v>
+        <v>517</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -7267,7 +7245,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -7275,7 +7253,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>533</v>
+        <v>519</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -7283,7 +7261,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>534</v>
+        <v>520</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -7291,7 +7269,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>535</v>
+        <v>521</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -7299,7 +7277,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>536</v>
+        <v>522</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -7334,7 +7312,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>537</v>
+        <v>523</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7350,7 +7328,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>538</v>
+        <v>524</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7366,7 +7344,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>539</v>
+        <v>525</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -7374,7 +7352,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>540</v>
+        <v>526</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -7446,7 +7424,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -7482,7 +7460,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7490,7 +7468,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7498,7 +7476,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7506,7 +7484,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -7514,7 +7492,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -7522,7 +7500,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -7530,7 +7508,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -7538,7 +7516,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -7546,7 +7524,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -7554,7 +7532,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -7562,7 +7540,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -7570,7 +7548,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -7578,7 +7556,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -7586,7 +7564,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -7594,7 +7572,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -7602,7 +7580,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -7610,7 +7588,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -7618,7 +7596,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -7626,7 +7604,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -7634,7 +7612,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -7642,7 +7620,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -7650,7 +7628,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -7658,7 +7636,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -7666,7 +7644,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -7674,7 +7652,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>570</v>
+        <v>556</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -7710,119 +7688,119 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="B3" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="B4" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="B5" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="B6" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="B8" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
       <c r="B10" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="B11" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="B12" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="B13" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="B14" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -7830,151 +7808,151 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="B17" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="B18" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="B19" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="B20" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="B21" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="B22" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="B23" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="B24" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="B25" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="B26" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="B27" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="B30" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="B31" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="B32" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="B33" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="B34" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -7982,298 +7960,298 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="B36" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="B37" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="B38" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="B39" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="B40" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="B41" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="B42" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="B43" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="B44" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="B45" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="B46" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="B47" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="B48" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="B49" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="B50" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="B51" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="B52" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="B53" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="B54" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="B55" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="B56" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="B57" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="B58" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="B59" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="B60" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="B61" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="B62" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="B63" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="B64" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="B65" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="B66" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="B67" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="B68" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
       <c r="B69" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
       <c r="B70" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="B71" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="B72" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -8334,7 +8312,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -8342,7 +8320,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -8350,7 +8328,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -8358,7 +8336,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -8366,7 +8344,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -8374,7 +8352,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -8382,7 +8360,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -8390,7 +8368,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -8398,7 +8376,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -8406,7 +8384,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -8414,7 +8392,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -8581,7 +8559,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -8669,7 +8647,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>579</v>
+        <v>565</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -8677,7 +8655,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>580</v>
+        <v>566</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -8685,7 +8663,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>581</v>
+        <v>567</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -8741,7 +8719,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>582</v>
+        <v>568</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -8749,7 +8727,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>583</v>
+        <v>569</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -8757,7 +8735,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>584</v>
+        <v>570</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -8765,7 +8743,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>585</v>
+        <v>571</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -8773,7 +8751,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>586</v>
+        <v>572</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -8781,7 +8759,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>587</v>
+        <v>573</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -8789,7 +8767,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>588</v>
+        <v>574</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -8797,7 +8775,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>589</v>
+        <v>575</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -8805,7 +8783,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>590</v>
+        <v>576</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -8813,7 +8791,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>591</v>
+        <v>577</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -8848,7 +8826,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -8856,7 +8834,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>506</v>
+        <v>492</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -8864,7 +8842,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -8872,7 +8850,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -8880,7 +8858,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -8888,7 +8866,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -8896,7 +8874,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -8904,7 +8882,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -8912,7 +8890,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -8920,7 +8898,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -8928,7 +8906,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -8936,7 +8914,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -8944,7 +8922,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>499</v>
+        <v>485</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -8952,7 +8930,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>498</v>
+        <v>484</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -8960,7 +8938,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>497</v>
+        <v>483</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -8968,7 +8946,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -8976,7 +8954,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>495</v>
+        <v>481</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -8984,7 +8962,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>494</v>
+        <v>480</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -8992,7 +8970,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>492</v>
+        <v>478</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -9000,7 +8978,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -9035,34 +9013,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
       <c r="B2" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="B3" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
       <c r="B4" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
       <c r="B5" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Further implementing the new freight data
* Fix more bugs in code
* Fix the code to produce figures
* Fix how we generate scenario files
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{21702BD4-B62F-4377-8B0D-0CBFF489688A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C081C7D1-F05C-4CA9-9176-0F931A2C59EF}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="13_ncr:1_{21702BD4-B62F-4377-8B0D-0CBFF489688A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87397E40-0BED-4CC4-8222-5B78E9196D02}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" firstSheet="3" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -42,6 +42,8 @@
     <sheet name="ITTI" sheetId="32" r:id="rId27"/>
     <sheet name="CTTI" sheetId="33" r:id="rId28"/>
     <sheet name="SCA" sheetId="37" r:id="rId29"/>
+    <sheet name="models_w_batteries" sheetId="40" r:id="rId30"/>
+    <sheet name="noit" sheetId="41" r:id="rId31"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RTI!$A$1:$B$1</definedName>
@@ -62,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="647">
   <si>
     <t>Full name</t>
   </si>
@@ -814,42 +816,12 @@
     <t>4 Coal + CCS</t>
   </si>
   <si>
-    <t>5 IGCC</t>
-  </si>
-  <si>
-    <t>6 IGCC + CCS</t>
-  </si>
-  <si>
     <t>7 CCGT</t>
   </si>
   <si>
     <t>8 CCGT + CCS</t>
   </si>
   <si>
-    <t>9 Solid Biomass</t>
-  </si>
-  <si>
-    <t>10 S Biomass CCS</t>
-  </si>
-  <si>
-    <t>11 BIGCC</t>
-  </si>
-  <si>
-    <t>12 BIGCC + CCS</t>
-  </si>
-  <si>
-    <t>13 Biogas</t>
-  </si>
-  <si>
-    <t>14 Biogas + CCS</t>
-  </si>
-  <si>
-    <t>15 Tidal</t>
-  </si>
-  <si>
-    <t>16 Large Hydro</t>
-  </si>
-  <si>
     <t>17 Onshore</t>
   </si>
   <si>
@@ -862,18 +834,6 @@
     <t>20 CSP</t>
   </si>
   <si>
-    <t>21 Geothermal</t>
-  </si>
-  <si>
-    <t>22 Wave</t>
-  </si>
-  <si>
-    <t>23 Fuel Cells</t>
-  </si>
-  <si>
-    <t>24 CHP</t>
-  </si>
-  <si>
     <t>4 Gas</t>
   </si>
   <si>
@@ -1991,6 +1951,60 @@
   </si>
   <si>
     <t>17 Battery cost ($/kWh)</t>
+  </si>
+  <si>
+    <t>FTT:P</t>
+  </si>
+  <si>
+    <t>FTT:Tr</t>
+  </si>
+  <si>
+    <t>FTT:Fr</t>
+  </si>
+  <si>
+    <t>5 Waste</t>
+  </si>
+  <si>
+    <t>6 Waste + CCS</t>
+  </si>
+  <si>
+    <t>9 OCGT</t>
+  </si>
+  <si>
+    <t>10 OCGT + CCS</t>
+  </si>
+  <si>
+    <t>11 Biomass</t>
+  </si>
+  <si>
+    <t>12 Biomass + CCS</t>
+  </si>
+  <si>
+    <t>13 Large Hydro</t>
+  </si>
+  <si>
+    <t>14 Pumped Hydro</t>
+  </si>
+  <si>
+    <t>15 Geothermal</t>
+  </si>
+  <si>
+    <t>16 Marine</t>
+  </si>
+  <si>
+    <t>21 Fuel cells / Turbine</t>
+  </si>
+  <si>
+    <t>22 Lithium-ion</t>
+  </si>
+  <si>
+    <t>V2G available fraction</t>
+  </si>
+  <si>
+    <t>V2G participation rate</t>
+  </si>
+  <si>
+    <t>Battery learning exponent</t>
   </si>
 </sst>
 </file>
@@ -3269,7 +3283,7 @@
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16" t="s">
-        <v>477</v>
+        <v>463</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3293,137 +3307,137 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="3" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="3" t="s">
-        <v>448</v>
+        <v>434</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="3" t="s">
-        <v>449</v>
+        <v>435</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>467</v>
+        <v>453</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="3" t="s">
-        <v>450</v>
+        <v>436</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="3" t="s">
-        <v>451</v>
+        <v>437</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>468</v>
+        <v>454</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="3" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="3" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>470</v>
+        <v>456</v>
       </c>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="3" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>471</v>
+        <v>457</v>
       </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="3" t="s">
-        <v>455</v>
+        <v>441</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="3" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="3" t="s">
-        <v>457</v>
+        <v>443</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="3" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>475</v>
+        <v>461</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="3" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>11</v>
@@ -3433,7 +3447,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="3" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>8</v>
@@ -3444,7 +3458,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="3" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>9</v>
@@ -3455,7 +3469,7 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="3" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>10</v>
@@ -3469,7 +3483,7 @@
         <v>12</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -3477,10 +3491,10 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6" t="s">
-        <v>572</v>
+        <v>558</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>573</v>
+        <v>559</v>
       </c>
       <c r="H30" s="3"/>
     </row>
@@ -3582,34 +3596,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
       <c r="B2" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="B3" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
       <c r="B4" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
       <c r="B5" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -12254,7 +12268,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>559</v>
+        <v>545</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -12286,7 +12300,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -12294,7 +12308,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>543</v>
+        <v>529</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -12302,7 +12316,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>542</v>
+        <v>528</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -12310,7 +12324,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>541</v>
+        <v>527</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -12318,7 +12332,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>540</v>
+        <v>526</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -12333,10 +12347,10 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C84BF1-D202-40D0-9C0C-F82CFDCF6C25}">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12386,7 +12400,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>250</v>
+        <v>632</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -12394,7 +12408,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>251</v>
+        <v>633</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -12402,7 +12416,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -12410,7 +12424,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -12418,7 +12432,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>254</v>
+        <v>634</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -12426,7 +12440,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>255</v>
+        <v>635</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -12434,7 +12448,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>256</v>
+        <v>636</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -12442,7 +12456,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>257</v>
+        <v>637</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -12450,7 +12464,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>258</v>
+        <v>638</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -12458,7 +12472,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>259</v>
+        <v>639</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -12466,7 +12480,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>260</v>
+        <v>640</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -12474,7 +12488,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>261</v>
+        <v>641</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -12482,7 +12496,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -12490,7 +12504,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -12498,7 +12512,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -12506,7 +12520,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -12514,7 +12528,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>266</v>
+        <v>642</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -12522,26 +12536,10 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>267</v>
+        <v>643</v>
       </c>
       <c r="B23">
         <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>268</v>
-      </c>
-      <c r="B24">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>269</v>
-      </c>
-      <c r="B25">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -12733,7 +12731,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>580</v>
+        <v>566</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -12750,7 +12748,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12768,7 +12766,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>581</v>
+        <v>567</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -12776,7 +12774,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>582</v>
+        <v>568</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -12824,7 +12822,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>583</v>
+        <v>569</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -12832,7 +12830,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>584</v>
+        <v>570</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -12840,7 +12838,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>635</v>
+        <v>621</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -12848,7 +12846,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>636</v>
+        <v>622</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -12856,7 +12854,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>637</v>
+        <v>623</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -12864,7 +12862,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>638</v>
+        <v>624</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -12872,7 +12870,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>639</v>
+        <v>625</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -12880,7 +12878,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>640</v>
+        <v>626</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -12888,7 +12886,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>641</v>
+        <v>627</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -12896,7 +12894,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>642</v>
+        <v>628</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -12928,7 +12926,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -12936,7 +12934,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -13176,7 +13174,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>560</v>
+        <v>546</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -13184,7 +13182,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>561</v>
+        <v>547</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -13192,7 +13190,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>562</v>
+        <v>548</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -13200,7 +13198,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>563</v>
+        <v>549</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -13224,7 +13222,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>564</v>
+        <v>550</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -13248,7 +13246,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -13288,7 +13286,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>566</v>
+        <v>552</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -13296,7 +13294,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -13304,7 +13302,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -13312,7 +13310,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -13320,7 +13318,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>570</v>
+        <v>556</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -13328,7 +13326,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -13362,106 +13360,106 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>514</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>508</v>
+        <v>494</v>
       </c>
       <c r="B2" t="s">
-        <v>511</v>
+        <v>497</v>
       </c>
       <c r="C2" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="B3" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
       <c r="C3" t="s">
-        <v>516</v>
+        <v>502</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="B4" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="C4" t="s">
-        <v>531</v>
+        <v>517</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>533</v>
+        <v>519</v>
       </c>
       <c r="B5" t="s">
-        <v>534</v>
+        <v>520</v>
       </c>
       <c r="C5" t="s">
-        <v>535</v>
+        <v>521</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="B6" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="C6" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
       <c r="B7" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="C7" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="B8" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="C8" t="s">
-        <v>519</v>
+        <v>505</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>524</v>
+        <v>510</v>
       </c>
       <c r="B9" t="s">
-        <v>527</v>
+        <v>513</v>
       </c>
       <c r="C9" t="s">
-        <v>520</v>
+        <v>506</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="B10" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="C10" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -15267,7 +15265,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15275,7 +15273,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -15283,7 +15281,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15291,7 +15289,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>481</v>
+        <v>467</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -15299,7 +15297,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -15307,7 +15305,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -15315,7 +15313,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -15323,7 +15321,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -15331,7 +15329,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -15339,7 +15337,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>487</v>
+        <v>473</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -15375,7 +15373,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15383,7 +15381,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>492</v>
+        <v>478</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -15391,7 +15389,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15399,7 +15397,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>494</v>
+        <v>480</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -15407,7 +15405,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>495</v>
+        <v>481</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -15415,7 +15413,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -15423,7 +15421,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>497</v>
+        <v>483</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -15431,7 +15429,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>498</v>
+        <v>484</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -15439,7 +15437,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>499</v>
+        <v>485</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -15447,7 +15445,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -15455,7 +15453,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -15463,7 +15461,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -15471,7 +15469,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -15506,7 +15504,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15522,7 +15520,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15538,7 +15536,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>506</v>
+        <v>492</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -15546,7 +15544,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -15618,7 +15616,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -15634,7 +15632,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15649,7 +15647,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>574</v>
+        <v>560</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15657,7 +15655,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>575</v>
+        <v>561</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -15665,7 +15663,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>579</v>
+        <v>565</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15673,7 +15671,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>576</v>
+        <v>562</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -15681,7 +15679,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>577</v>
+        <v>563</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -15689,7 +15687,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>578</v>
+        <v>644</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -15697,7 +15695,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>578</v>
+        <v>645</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -15705,7 +15703,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>578</v>
+        <v>646</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -15713,7 +15711,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -15721,7 +15719,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -15729,7 +15727,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -15737,7 +15735,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -15745,7 +15743,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -15753,7 +15751,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -15789,7 +15787,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15797,7 +15795,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -15805,7 +15803,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15813,7 +15811,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -15821,7 +15819,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -15829,7 +15827,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -15837,7 +15835,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -15845,7 +15843,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -15853,7 +15851,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -15861,7 +15859,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -15869,7 +15867,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -15877,7 +15875,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -15885,7 +15883,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -15893,7 +15891,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -15901,7 +15899,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -15909,7 +15907,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -15917,7 +15915,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -15925,7 +15923,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -15933,7 +15931,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -15941,7 +15939,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -15949,7 +15947,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -15957,7 +15955,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -15965,7 +15963,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -15973,7 +15971,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>538</v>
+        <v>524</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -15981,10 +15979,112 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>539</v>
+        <v>525</v>
       </c>
       <c r="B26">
         <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CB11C9-8F34-4153-8146-11441D7966B6}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>630</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>631</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BCCAA29-949C-4929-B734-81A6430E50F2}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -16017,119 +16117,119 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="B3" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="B4" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="B5" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="B6" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="B8" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
       <c r="B10" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="B11" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="B12" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="B13" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="B14" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -16137,151 +16237,151 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="B17" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="B18" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="B19" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="B20" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="B21" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="B22" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="B23" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="B24" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="B25" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="B26" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="B27" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="B30" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="B31" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="B32" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="B33" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="B34" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -16289,298 +16389,298 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="B36" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="B37" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="B38" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="B39" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="B40" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="B41" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="B42" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="B43" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="B44" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="B45" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="B46" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="B47" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="B48" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="B49" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="B50" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="B51" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="B52" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="B53" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="B54" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="B55" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="B56" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="B57" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="B58" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="B59" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="B60" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="B61" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="B62" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="B63" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="B64" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="B65" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="B66" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="B67" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="B68" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
       <c r="B69" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
       <c r="B70" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="B71" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>536</v>
+        <v>522</v>
       </c>
       <c r="B72" t="s">
-        <v>537</v>
+        <v>523</v>
       </c>
     </row>
   </sheetData>
@@ -16641,7 +16741,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -16649,7 +16749,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -16657,7 +16757,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -16665,7 +16765,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -16673,7 +16773,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -16681,7 +16781,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -16689,7 +16789,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -16697,7 +16797,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -16705,7 +16805,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -16713,7 +16813,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -16721,7 +16821,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -16888,7 +16988,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>545</v>
+        <v>531</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -16976,7 +17076,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>546</v>
+        <v>532</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -16984,7 +17084,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -16992,7 +17092,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>548</v>
+        <v>534</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -17048,7 +17148,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>549</v>
+        <v>535</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -17056,7 +17156,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -17064,7 +17164,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>551</v>
+        <v>537</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -17072,7 +17172,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>552</v>
+        <v>538</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -17080,7 +17180,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>553</v>
+        <v>539</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -17088,7 +17188,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -17096,7 +17196,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -17104,7 +17204,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>556</v>
+        <v>542</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -17112,7 +17212,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>557</v>
+        <v>543</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -17120,7 +17220,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -17155,7 +17255,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>621</v>
+        <v>607</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -17163,7 +17263,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>585</v>
+        <v>571</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -17171,7 +17271,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>586</v>
+        <v>572</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -17179,7 +17279,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>587</v>
+        <v>573</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -17187,7 +17287,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>588</v>
+        <v>574</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -17195,7 +17295,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -17203,7 +17303,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>589</v>
+        <v>575</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -17211,7 +17311,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>590</v>
+        <v>576</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -17219,7 +17319,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>591</v>
+        <v>577</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -17227,7 +17327,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>592</v>
+        <v>578</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -17235,7 +17335,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>623</v>
+        <v>609</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -17243,7 +17343,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -17251,7 +17351,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>594</v>
+        <v>580</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -17259,7 +17359,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>595</v>
+        <v>581</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -17267,7 +17367,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>596</v>
+        <v>582</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -17275,7 +17375,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>624</v>
+        <v>610</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -17283,7 +17383,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>597</v>
+        <v>583</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -17291,7 +17391,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>598</v>
+        <v>584</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -17299,7 +17399,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>599</v>
+        <v>585</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -17307,7 +17407,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>600</v>
+        <v>586</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -17315,7 +17415,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>625</v>
+        <v>611</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -17323,7 +17423,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>601</v>
+        <v>587</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -17331,7 +17431,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>602</v>
+        <v>588</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -17339,7 +17439,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>603</v>
+        <v>589</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -17347,7 +17447,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>604</v>
+        <v>590</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -17355,7 +17455,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -17363,7 +17463,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>605</v>
+        <v>591</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -17371,7 +17471,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>606</v>
+        <v>592</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -17379,7 +17479,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>607</v>
+        <v>593</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -17387,7 +17487,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>608</v>
+        <v>594</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -17395,7 +17495,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>627</v>
+        <v>613</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -17403,7 +17503,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>609</v>
+        <v>595</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -17411,7 +17511,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>610</v>
+        <v>596</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -17419,7 +17519,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>611</v>
+        <v>597</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -17427,7 +17527,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>612</v>
+        <v>598</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -17435,7 +17535,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>628</v>
+        <v>614</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -17443,7 +17543,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>613</v>
+        <v>599</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -17451,7 +17551,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>614</v>
+        <v>600</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -17459,7 +17559,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -17467,7 +17567,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -17475,7 +17575,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>629</v>
+        <v>615</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -17483,7 +17583,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>617</v>
+        <v>603</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -17491,7 +17591,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>618</v>
+        <v>604</v>
       </c>
       <c r="B44">
         <v>43</v>
@@ -17499,7 +17599,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>619</v>
+        <v>605</v>
       </c>
       <c r="B45">
         <v>44</v>
@@ -17507,7 +17607,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -17541,7 +17641,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -17549,7 +17649,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -17557,7 +17657,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>632</v>
+        <v>618</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -17565,7 +17665,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>633</v>
+        <v>619</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -17573,7 +17673,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>634</v>
+        <v>620</v>
       </c>
       <c r="B6">
         <v>5</v>

</xml_diff>

<commit_message>
Added carbon costs and restraints on capacity growth
Included static emission factors in the cost matrix.
Added carbon price variable to calculate carbon costs.
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{5CED7FD4-CBE8-4FF4-A1F6-D31781E59327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55F4631A-06B2-4063-A72D-01FFB3461402}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="14" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="14" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -8088,7 +8088,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
start the gamma value automation on this branch
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work profile\OneDrive - University of Exeter\Documents\GitHub\FTT_StandAlone\Utilities\titles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="13_ncr:1_{21702BD4-B62F-4377-8B0D-0CBFF489688A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87397E40-0BED-4CC4-8222-5B78E9196D02}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07137CA-B164-4F50-99A2-0E47A14DBA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="663">
   <si>
     <t>Full name</t>
   </si>
@@ -2005,6 +2005,54 @@
   </si>
   <si>
     <t>Battery learning exponent</t>
+  </si>
+  <si>
+    <t>shares_roc_var</t>
+  </si>
+  <si>
+    <t>tech_var</t>
+  </si>
+  <si>
+    <t>histend_var</t>
+  </si>
+  <si>
+    <t>MSRC</t>
+  </si>
+  <si>
+    <t>MEWG</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>HEWF</t>
+  </si>
+  <si>
+    <t>TEWS</t>
+  </si>
+  <si>
+    <t>shares_var</t>
+  </si>
+  <si>
+    <t>MEWS</t>
+  </si>
+  <si>
+    <t>HEWS</t>
+  </si>
+  <si>
+    <t>IWS1</t>
+  </si>
+  <si>
+    <t>IWS2</t>
+  </si>
+  <si>
+    <t>IWS3</t>
+  </si>
+  <si>
+    <t>IWS4</t>
+  </si>
+  <si>
+    <t>IWS5</t>
   </si>
 </sst>
 </file>
@@ -12747,7 +12795,7 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -13340,10 +13388,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AE06A4-CDB3-4DA5-AA93-26CDCBA71A9A}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13352,7 +13400,7 @@
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13362,8 +13410,20 @@
       <c r="C1" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>655</v>
+      </c>
+      <c r="E1" t="s">
+        <v>647</v>
+      </c>
+      <c r="F1" t="s">
+        <v>648</v>
+      </c>
+      <c r="G1" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>494</v>
       </c>
@@ -13373,8 +13433,20 @@
       <c r="C2" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>656</v>
+      </c>
+      <c r="E2" t="s">
+        <v>650</v>
+      </c>
+      <c r="F2" t="s">
+        <v>440</v>
+      </c>
+      <c r="G2" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>496</v>
       </c>
@@ -13384,8 +13456,20 @@
       <c r="C3" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>657</v>
+      </c>
+      <c r="E3" t="s">
+        <v>652</v>
+      </c>
+      <c r="F3" t="s">
+        <v>443</v>
+      </c>
+      <c r="G3" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>516</v>
       </c>
@@ -13395,8 +13479,20 @@
       <c r="C4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>654</v>
+      </c>
+      <c r="E4" t="s">
+        <v>652</v>
+      </c>
+      <c r="F4" t="s">
+        <v>436</v>
+      </c>
+      <c r="G4" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>519</v>
       </c>
@@ -13406,8 +13502,20 @@
       <c r="C5" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>652</v>
+      </c>
+      <c r="E5" t="s">
+        <v>652</v>
+      </c>
+      <c r="F5" t="s">
+        <v>652</v>
+      </c>
+      <c r="G5" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>495</v>
       </c>
@@ -13417,8 +13525,20 @@
       <c r="C6" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>658</v>
+      </c>
+      <c r="E6" t="s">
+        <v>652</v>
+      </c>
+      <c r="F6" t="s">
+        <v>652</v>
+      </c>
+      <c r="G6" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>508</v>
       </c>
@@ -13428,8 +13548,20 @@
       <c r="C7" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>659</v>
+      </c>
+      <c r="E7" t="s">
+        <v>652</v>
+      </c>
+      <c r="F7" t="s">
+        <v>652</v>
+      </c>
+      <c r="G7" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>509</v>
       </c>
@@ -13439,8 +13571,20 @@
       <c r="C8" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>660</v>
+      </c>
+      <c r="E8" t="s">
+        <v>652</v>
+      </c>
+      <c r="F8" t="s">
+        <v>652</v>
+      </c>
+      <c r="G8" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>510</v>
       </c>
@@ -13450,8 +13594,20 @@
       <c r="C9" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>661</v>
+      </c>
+      <c r="E9" t="s">
+        <v>652</v>
+      </c>
+      <c r="F9" t="s">
+        <v>652</v>
+      </c>
+      <c r="G9" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>515</v>
       </c>
@@ -13460,6 +13616,18 @@
       </c>
       <c r="C10" t="s">
         <v>507</v>
+      </c>
+      <c r="D10" t="s">
+        <v>662</v>
+      </c>
+      <c r="E10" t="s">
+        <v>652</v>
+      </c>
+      <c r="F10" t="s">
+        <v>652</v>
+      </c>
+      <c r="G10" t="s">
+        <v>652</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first round of testing
Fixed a couple of issues. Can now run it with the other models too. Probably more issues to be found.
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{F07137CA-B164-4F50-99A2-0E47A14DBA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7318786C-93DA-4D16-8699-3AA23764A9FA}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{F07137CA-B164-4F50-99A2-0E47A14DBA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68165DA6-4263-400E-8DA5-BE6560A28CD2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="664">
   <si>
     <t>Full name</t>
   </si>
@@ -2047,6 +2047,15 @@
   </si>
   <si>
     <t>IWS5</t>
+  </si>
+  <si>
+    <t>ZEWS</t>
+  </si>
+  <si>
+    <t>FTTI</t>
+  </si>
+  <si>
+    <t>RFLZ</t>
   </si>
 </sst>
 </file>
@@ -13385,7 +13394,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13485,13 +13494,13 @@
         <v>521</v>
       </c>
       <c r="D5" t="s">
-        <v>650</v>
+        <v>661</v>
       </c>
       <c r="E5" t="s">
-        <v>650</v>
+        <v>662</v>
       </c>
       <c r="F5" t="s">
-        <v>650</v>
+        <v>663</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Make gamma 1D, improve automation
Further changing the step size of the automation algorithm, for improved speed and accuracy.
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{F07137CA-B164-4F50-99A2-0E47A14DBA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68165DA6-4263-400E-8DA5-BE6560A28CD2}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{D54A4C60-6278-4785-934E-4CE5636D7FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67C74EF1-CE7B-42C6-8398-65E37E0F5671}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="671">
   <si>
     <t>Full name</t>
   </si>
@@ -438,9 +438,6 @@
     <t>12 Cap_F (Mpkm/kseats-y)</t>
   </si>
   <si>
-    <t>13 Gam (initial)</t>
-  </si>
-  <si>
     <t>15 Seats/Veh</t>
   </si>
   <si>
@@ -1764,9 +1761,6 @@
     <t>Starting degradation</t>
   </si>
   <si>
-    <t>21 Gamma ($/MWh)</t>
-  </si>
-  <si>
     <t>1 Purchase cost (USD/veh)</t>
   </si>
   <si>
@@ -1932,9 +1926,6 @@
     <t>10 Loads (t or passengers/veh)</t>
   </si>
   <si>
-    <t>11 Gamma value</t>
-  </si>
-  <si>
     <t>12 CO2 emissions (gCO2/km)</t>
   </si>
   <si>
@@ -2056,6 +2047,36 @@
   </si>
   <si>
     <t>RFLZ</t>
+  </si>
+  <si>
+    <t>Cost_var</t>
+  </si>
+  <si>
+    <t>Gamma_ind</t>
+  </si>
+  <si>
+    <t>BCET</t>
+  </si>
+  <si>
+    <t>BHTC</t>
+  </si>
+  <si>
+    <t>BTTC</t>
+  </si>
+  <si>
+    <t>BZTC</t>
+  </si>
+  <si>
+    <t>13 Gamma</t>
+  </si>
+  <si>
+    <t>11 Gamma</t>
+  </si>
+  <si>
+    <t>21 Storage</t>
+  </si>
+  <si>
+    <t>22 Gamma</t>
   </si>
 </sst>
 </file>
@@ -3334,7 +3355,7 @@
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3358,137 +3379,137 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>11</v>
@@ -3498,7 +3519,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>8</v>
@@ -3509,7 +3530,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>9</v>
@@ -3520,7 +3541,7 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>10</v>
@@ -3534,7 +3555,7 @@
         <v>12</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -3542,10 +3563,10 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>558</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>559</v>
       </c>
       <c r="H30" s="3"/>
     </row>
@@ -3647,34 +3668,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -12196,7 +12217,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12311,7 +12332,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>667</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -12319,7 +12340,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -12327,7 +12348,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -12335,7 +12356,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -12343,7 +12364,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -12351,7 +12372,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -12359,7 +12380,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -12367,7 +12388,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -12375,7 +12396,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -12383,7 +12404,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -12419,7 +12440,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -12427,7 +12448,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -12435,7 +12456,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -12443,7 +12464,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -12451,7 +12472,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -12459,7 +12480,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -12467,7 +12488,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -12475,7 +12496,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -12483,7 +12504,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -12491,7 +12512,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -12499,7 +12520,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -12507,7 +12528,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -12515,7 +12536,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -12523,7 +12544,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -12531,7 +12552,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -12539,7 +12560,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -12547,7 +12568,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -12555,7 +12576,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -12563,7 +12584,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -12571,7 +12592,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -12579,7 +12600,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -12587,7 +12608,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -12601,10 +12622,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C01FE79-1B64-410C-BFB3-7EE7C4F3E8BE}">
   <sheetPr codeName="Sheet13"/>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12622,7 +12643,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -12630,7 +12651,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -12638,7 +12659,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -12646,7 +12667,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -12654,7 +12675,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -12662,7 +12683,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -12670,7 +12691,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -12678,7 +12699,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -12686,7 +12707,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -12694,7 +12715,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -12702,7 +12723,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -12710,7 +12731,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -12718,7 +12739,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -12726,7 +12747,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -12734,7 +12755,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -12742,7 +12763,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -12750,7 +12771,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -12758,7 +12779,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -12766,7 +12787,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -12774,7 +12795,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -12782,10 +12803,18 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>566</v>
+        <v>669</v>
       </c>
       <c r="B22">
         <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>670</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -12799,7 +12828,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12817,7 +12846,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -12825,7 +12854,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -12873,7 +12902,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -12881,7 +12910,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -12889,7 +12918,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -12897,7 +12926,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>622</v>
+        <v>668</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -12905,7 +12934,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -12913,7 +12942,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -12921,7 +12950,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -12929,7 +12958,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -12937,7 +12966,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -12945,7 +12974,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -12977,7 +13006,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -12985,7 +13014,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -13017,7 +13046,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -13025,7 +13054,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -13033,7 +13062,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -13041,7 +13070,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -13049,7 +13078,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -13057,7 +13086,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -13093,7 +13122,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -13101,7 +13130,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -13109,7 +13138,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -13117,7 +13146,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -13125,7 +13154,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -13133,7 +13162,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -13141,7 +13170,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -13149,7 +13178,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -13157,7 +13186,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -13165,7 +13194,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -13173,7 +13202,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -13181,7 +13210,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -13189,7 +13218,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -13225,7 +13254,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -13233,7 +13262,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -13241,7 +13270,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -13249,7 +13278,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -13257,7 +13286,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -13265,7 +13294,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -13273,7 +13302,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -13281,7 +13310,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -13289,7 +13318,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -13297,7 +13326,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -13305,7 +13334,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -13313,7 +13342,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -13321,7 +13350,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -13329,7 +13358,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -13337,7 +13366,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -13345,7 +13374,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -13353,7 +13382,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -13361,7 +13390,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -13369,7 +13398,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -13377,7 +13406,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -13391,19 +13420,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AE06A4-CDB3-4DA5-AA93-26CDCBA71A9A}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13411,196 +13441,256 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>661</v>
+      </c>
+      <c r="D1" t="s">
+        <v>662</v>
+      </c>
+      <c r="E1" t="s">
+        <v>499</v>
+      </c>
+      <c r="F1" t="s">
+        <v>650</v>
+      </c>
+      <c r="G1" t="s">
+        <v>644</v>
+      </c>
+      <c r="H1" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>493</v>
+      </c>
+      <c r="B2" t="s">
+        <v>496</v>
+      </c>
+      <c r="C2" t="s">
+        <v>663</v>
+      </c>
+      <c r="D2">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
         <v>500</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F2" t="s">
+        <v>651</v>
+      </c>
+      <c r="G2" t="s">
+        <v>439</v>
+      </c>
+      <c r="H2" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B3" t="s">
+        <v>497</v>
+      </c>
+      <c r="C3" t="s">
+        <v>664</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>501</v>
+      </c>
+      <c r="F3" t="s">
+        <v>652</v>
+      </c>
+      <c r="G3" t="s">
+        <v>442</v>
+      </c>
+      <c r="H3" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>515</v>
+      </c>
+      <c r="B4" t="s">
+        <v>517</v>
+      </c>
+      <c r="C4" t="s">
+        <v>665</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>516</v>
+      </c>
+      <c r="F4" t="s">
+        <v>649</v>
+      </c>
+      <c r="G4" t="s">
+        <v>435</v>
+      </c>
+      <c r="H4" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>518</v>
+      </c>
+      <c r="B5" t="s">
+        <v>519</v>
+      </c>
+      <c r="C5" t="s">
+        <v>666</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>520</v>
+      </c>
+      <c r="F5" t="s">
+        <v>658</v>
+      </c>
+      <c r="G5" t="s">
+        <v>659</v>
+      </c>
+      <c r="H5" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>494</v>
+      </c>
+      <c r="B6" t="s">
+        <v>498</v>
+      </c>
+      <c r="C6" t="s">
+        <v>647</v>
+      </c>
+      <c r="D6" t="s">
+        <v>647</v>
+      </c>
+      <c r="E6" t="s">
+        <v>502</v>
+      </c>
+      <c r="F6" t="s">
         <v>653</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G6" t="s">
         <v>647</v>
       </c>
-      <c r="F1" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>494</v>
-      </c>
-      <c r="B2" t="s">
-        <v>497</v>
-      </c>
-      <c r="C2" t="s">
-        <v>501</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="H6" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>507</v>
+      </c>
+      <c r="B7" t="s">
+        <v>510</v>
+      </c>
+      <c r="C7" t="s">
+        <v>647</v>
+      </c>
+      <c r="D7" t="s">
+        <v>647</v>
+      </c>
+      <c r="E7" t="s">
+        <v>503</v>
+      </c>
+      <c r="F7" t="s">
         <v>654</v>
       </c>
-      <c r="E2" t="s">
-        <v>440</v>
-      </c>
-      <c r="F2" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>496</v>
-      </c>
-      <c r="B3" t="s">
-        <v>498</v>
-      </c>
-      <c r="C3" t="s">
-        <v>502</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="G7" t="s">
+        <v>647</v>
+      </c>
+      <c r="H7" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>508</v>
+      </c>
+      <c r="B8" t="s">
+        <v>511</v>
+      </c>
+      <c r="C8" t="s">
+        <v>647</v>
+      </c>
+      <c r="D8" t="s">
+        <v>647</v>
+      </c>
+      <c r="E8" t="s">
+        <v>504</v>
+      </c>
+      <c r="F8" t="s">
         <v>655</v>
       </c>
-      <c r="E3" t="s">
-        <v>443</v>
-      </c>
-      <c r="F3" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>516</v>
-      </c>
-      <c r="B4" t="s">
-        <v>518</v>
-      </c>
-      <c r="C4" t="s">
-        <v>517</v>
-      </c>
-      <c r="D4" t="s">
-        <v>652</v>
-      </c>
-      <c r="E4" t="s">
-        <v>436</v>
-      </c>
-      <c r="F4" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>519</v>
-      </c>
-      <c r="B5" t="s">
-        <v>520</v>
-      </c>
-      <c r="C5" t="s">
-        <v>521</v>
-      </c>
-      <c r="D5" t="s">
-        <v>661</v>
-      </c>
-      <c r="E5" t="s">
-        <v>662</v>
-      </c>
-      <c r="F5" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>495</v>
-      </c>
-      <c r="B6" t="s">
-        <v>499</v>
-      </c>
-      <c r="C6" t="s">
-        <v>503</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="G8" t="s">
+        <v>647</v>
+      </c>
+      <c r="H8" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B9" t="s">
+        <v>512</v>
+      </c>
+      <c r="C9" t="s">
+        <v>647</v>
+      </c>
+      <c r="D9" t="s">
+        <v>647</v>
+      </c>
+      <c r="E9" t="s">
+        <v>505</v>
+      </c>
+      <c r="F9" t="s">
         <v>656</v>
       </c>
-      <c r="E6" t="s">
-        <v>650</v>
-      </c>
-      <c r="F6" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>508</v>
-      </c>
-      <c r="B7" t="s">
-        <v>511</v>
-      </c>
-      <c r="C7" t="s">
-        <v>504</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="G9" t="s">
+        <v>647</v>
+      </c>
+      <c r="H9" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>514</v>
+      </c>
+      <c r="B10" t="s">
+        <v>513</v>
+      </c>
+      <c r="C10" t="s">
+        <v>647</v>
+      </c>
+      <c r="D10" t="s">
+        <v>647</v>
+      </c>
+      <c r="E10" t="s">
+        <v>506</v>
+      </c>
+      <c r="F10" t="s">
         <v>657</v>
       </c>
-      <c r="E7" t="s">
-        <v>650</v>
-      </c>
-      <c r="F7" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>509</v>
-      </c>
-      <c r="B8" t="s">
-        <v>512</v>
-      </c>
-      <c r="C8" t="s">
-        <v>505</v>
-      </c>
-      <c r="D8" t="s">
-        <v>658</v>
-      </c>
-      <c r="E8" t="s">
-        <v>650</v>
-      </c>
-      <c r="F8" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>510</v>
-      </c>
-      <c r="B9" t="s">
-        <v>513</v>
-      </c>
-      <c r="C9" t="s">
-        <v>506</v>
-      </c>
-      <c r="D9" t="s">
-        <v>659</v>
-      </c>
-      <c r="E9" t="s">
-        <v>650</v>
-      </c>
-      <c r="F9" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>515</v>
-      </c>
-      <c r="B10" t="s">
-        <v>514</v>
-      </c>
-      <c r="C10" t="s">
-        <v>507</v>
-      </c>
-      <c r="D10" t="s">
-        <v>660</v>
-      </c>
-      <c r="E10" t="s">
-        <v>650</v>
-      </c>
-      <c r="F10" t="s">
-        <v>650</v>
+      <c r="G10" t="s">
+        <v>647</v>
+      </c>
+      <c r="H10" t="s">
+        <v>647</v>
       </c>
     </row>
   </sheetData>
@@ -13633,7 +13723,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -13641,7 +13731,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -13649,7 +13739,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -13657,7 +13747,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -13665,7 +13755,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -13673,7 +13763,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -13681,7 +13771,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -13689,7 +13779,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -13697,7 +13787,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -13705,7 +13795,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -13713,7 +13803,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -13721,7 +13811,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -13729,7 +13819,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -13737,7 +13827,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -13745,7 +13835,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -13753,7 +13843,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -13761,7 +13851,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -13769,7 +13859,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -13777,7 +13867,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -13785,7 +13875,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -13793,7 +13883,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -13801,7 +13891,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -13809,7 +13899,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -13817,7 +13907,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -13853,7 +13943,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -13861,7 +13951,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -13869,7 +13959,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -13877,7 +13967,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -13885,7 +13975,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -13893,7 +13983,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -13901,7 +13991,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -13909,7 +13999,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -13917,7 +14007,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -13925,7 +14015,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -13933,7 +14023,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -13941,7 +14031,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -13949,7 +14039,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -13957,7 +14047,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -13965,7 +14055,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -13973,7 +14063,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -13981,7 +14071,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -13989,7 +14079,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -13997,7 +14087,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -14005,7 +14095,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -14013,7 +14103,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -14021,7 +14111,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -14029,7 +14119,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -14037,7 +14127,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -14045,7 +14135,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -14053,7 +14143,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -14061,7 +14151,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -14069,7 +14159,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -14077,7 +14167,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -14085,7 +14175,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -14093,7 +14183,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -14101,7 +14191,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -14109,7 +14199,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -14117,7 +14207,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -14125,7 +14215,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -14133,7 +14223,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -14141,7 +14231,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -14149,7 +14239,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -14157,7 +14247,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -14165,7 +14255,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -14173,7 +14263,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -14181,7 +14271,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -14189,7 +14279,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B44">
         <v>43</v>
@@ -15406,7 +15496,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15414,7 +15504,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -15422,7 +15512,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15430,7 +15520,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -15438,7 +15528,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -15446,7 +15536,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -15454,7 +15544,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -15462,7 +15552,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -15470,7 +15560,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -15478,7 +15568,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -15514,7 +15604,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15522,7 +15612,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -15530,7 +15620,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15538,7 +15628,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -15546,7 +15636,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -15554,7 +15644,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -15562,7 +15652,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -15570,7 +15660,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -15578,7 +15668,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -15586,7 +15676,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -15594,7 +15684,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -15602,7 +15692,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -15610,7 +15700,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -15645,7 +15735,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15653,7 +15743,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -15661,7 +15751,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15669,7 +15759,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -15677,7 +15767,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -15685,7 +15775,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -15693,7 +15783,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -15701,7 +15791,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -15709,7 +15799,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -15717,7 +15807,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -15725,7 +15815,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -15733,7 +15823,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -15741,7 +15831,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -15749,7 +15839,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -15757,7 +15847,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -15788,7 +15878,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15796,7 +15886,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -15804,7 +15894,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15812,7 +15902,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -15820,7 +15910,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -15828,7 +15918,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -15836,7 +15926,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -15844,7 +15934,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -15852,7 +15942,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -15860,7 +15950,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -15868,7 +15958,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -15876,7 +15966,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -15884,7 +15974,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -15892,7 +15982,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -15928,7 +16018,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15936,7 +16026,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -15944,7 +16034,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15952,7 +16042,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -15960,7 +16050,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -15968,7 +16058,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -15976,7 +16066,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -15984,7 +16074,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -15992,7 +16082,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -16000,7 +16090,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -16008,7 +16098,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -16016,7 +16106,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -16024,7 +16114,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -16032,7 +16122,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -16040,7 +16130,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -16048,7 +16138,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -16056,7 +16146,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -16064,7 +16154,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -16072,7 +16162,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -16080,7 +16170,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -16088,7 +16178,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -16096,7 +16186,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -16104,7 +16194,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -16112,7 +16202,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -16120,7 +16210,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -16151,7 +16241,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -16159,7 +16249,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -16167,7 +16257,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -16258,119 +16348,119 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -16378,151 +16468,151 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B27" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B31" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B32" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -16530,298 +16620,298 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B36" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B37" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B38" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B39" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B40" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B41" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B43" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B45" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B46" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B47" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B49" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B50" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B51" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B52" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B53" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B54" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B55" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B56" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B57" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B58" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B59" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B60" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B61" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B62" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B63" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B64" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B65" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B66" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B67" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B68" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B69" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B70" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B71" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>521</v>
+      </c>
+      <c r="B72" t="s">
         <v>522</v>
-      </c>
-      <c r="B72" t="s">
-        <v>523</v>
       </c>
     </row>
   </sheetData>
@@ -16858,7 +16948,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -16866,7 +16956,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -16874,7 +16964,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -16882,7 +16972,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -16890,7 +16980,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -16898,7 +16988,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -16906,7 +16996,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -16914,7 +17004,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -16922,7 +17012,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -16930,7 +17020,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -16938,7 +17028,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -16946,7 +17036,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -16954,7 +17044,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -16962,7 +17052,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -17129,7 +17219,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -17217,7 +17307,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -17225,7 +17315,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -17233,7 +17323,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -17289,7 +17379,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -17297,7 +17387,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -17305,7 +17395,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -17313,7 +17403,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -17321,7 +17411,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -17329,7 +17419,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -17337,7 +17427,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -17345,7 +17435,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -17353,7 +17443,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -17361,7 +17451,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -17396,7 +17486,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -17404,7 +17494,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -17412,7 +17502,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -17420,7 +17510,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -17428,7 +17518,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -17436,7 +17526,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -17444,7 +17534,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -17452,7 +17542,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -17460,7 +17550,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -17468,7 +17558,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -17476,7 +17566,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -17484,7 +17574,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -17492,7 +17582,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -17500,7 +17590,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -17508,7 +17598,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -17516,7 +17606,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -17524,7 +17614,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -17532,7 +17622,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -17540,7 +17630,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -17548,7 +17638,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -17556,7 +17646,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -17564,7 +17654,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -17572,7 +17662,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -17580,7 +17670,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -17588,7 +17678,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -17596,7 +17686,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -17604,7 +17694,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -17612,7 +17702,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -17620,7 +17710,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -17628,7 +17718,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -17636,7 +17726,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -17644,7 +17734,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -17652,7 +17742,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -17660,7 +17750,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -17668,7 +17758,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -17676,7 +17766,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -17684,7 +17774,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -17692,7 +17782,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -17700,7 +17790,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -17708,7 +17798,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -17716,7 +17806,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -17724,7 +17814,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -17732,7 +17822,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B44">
         <v>43</v>
@@ -17740,7 +17830,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B45">
         <v>44</v>
@@ -17748,7 +17838,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -17782,7 +17872,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -17790,7 +17880,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -17798,7 +17888,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -17806,7 +17896,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -17814,7 +17904,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -17823,4 +17913,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{912a5d77-fb98-4eee-af32-1334d8f04a53}" enabled="0" method="" siteId="{912a5d77-fb98-4eee-af32-1334d8f04a53}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Fix error cost curves
Fix what happens when TP is reached
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -12625,7 +12625,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix error with replacement time
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work profile\OneDrive - University of Exeter\Documents\GitHub\FTT_StandAlone\Utilities\titles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{D54A4C60-6278-4785-934E-4CE5636D7FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67C74EF1-CE7B-42C6-8398-65E37E0F5671}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777B2733-6EDE-4DF4-88DD-3A6AAE61BFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="675" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -573,9 +573,6 @@
     <t>5 Lifetime</t>
   </si>
   <si>
-    <t>6 Leadtime</t>
-  </si>
-  <si>
     <t>7 Learning rate</t>
   </si>
   <si>
@@ -1701,9 +1698,6 @@
     <t>14 CO2Emissions</t>
   </si>
   <si>
-    <t>1 Inv cost mean (EUR/Kw)</t>
-  </si>
-  <si>
     <t>2 Inv Cost SD</t>
   </si>
   <si>
@@ -2077,6 +2071,12 @@
   </si>
   <si>
     <t>22 Gamma</t>
+  </si>
+  <si>
+    <t>6 Replacetime</t>
+  </si>
+  <si>
+    <t>1 Inv cost mean (EUR/kW)</t>
   </si>
 </sst>
 </file>
@@ -3355,7 +3355,7 @@
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3379,137 +3379,137 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>11</v>
@@ -3519,7 +3519,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>8</v>
@@ -3530,7 +3530,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>9</v>
@@ -3541,7 +3541,7 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>10</v>
@@ -3555,7 +3555,7 @@
         <v>12</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -3563,10 +3563,10 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="H30" s="3"/>
     </row>
@@ -3668,34 +3668,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -12332,7 +12332,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -12340,7 +12340,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -12372,7 +12372,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -12380,7 +12380,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -12388,7 +12388,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -12396,7 +12396,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -12404,7 +12404,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -12440,7 +12440,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -12448,7 +12448,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -12456,7 +12456,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -12464,7 +12464,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -12472,7 +12472,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -12480,7 +12480,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -12488,7 +12488,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -12496,7 +12496,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -12504,7 +12504,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -12512,7 +12512,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -12520,7 +12520,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -12528,7 +12528,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -12536,7 +12536,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -12544,7 +12544,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -12552,7 +12552,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -12560,7 +12560,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -12568,7 +12568,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -12576,7 +12576,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -12584,7 +12584,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -12592,7 +12592,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -12600,7 +12600,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -12608,7 +12608,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -12624,7 +12624,7 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -12803,7 +12803,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -12811,7 +12811,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -12846,7 +12846,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -12854,7 +12854,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -12902,7 +12902,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -12910,7 +12910,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -12918,7 +12918,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -12926,7 +12926,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -12934,7 +12934,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -12942,7 +12942,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -12950,7 +12950,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -12958,7 +12958,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -12966,7 +12966,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -12974,7 +12974,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -13006,7 +13006,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -13014,7 +13014,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -13234,8 +13234,8 @@
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13254,7 +13254,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>545</v>
+        <v>670</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -13262,7 +13262,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -13270,7 +13270,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -13278,7 +13278,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -13294,7 +13294,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>669</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -13302,7 +13302,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -13310,7 +13310,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -13318,7 +13318,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -13326,7 +13326,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -13334,7 +13334,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -13342,7 +13342,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -13350,7 +13350,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -13358,7 +13358,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -13366,7 +13366,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -13374,7 +13374,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -13382,7 +13382,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -13390,7 +13390,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -13398,7 +13398,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -13406,7 +13406,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -13441,256 +13441,256 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="G1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="H1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C2" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="D2">
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F2" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="G2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H2" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C3" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D3">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F3" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="G3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H3" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C4" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D4">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F4" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="G4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H4" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>517</v>
+      </c>
+      <c r="B5" t="s">
         <v>518</v>
       </c>
-      <c r="B5" t="s">
-        <v>519</v>
-      </c>
       <c r="C5" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F5" t="s">
+        <v>656</v>
+      </c>
+      <c r="G5" t="s">
+        <v>657</v>
+      </c>
+      <c r="H5" t="s">
         <v>658</v>
-      </c>
-      <c r="G5" t="s">
-        <v>659</v>
-      </c>
-      <c r="H5" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="E6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="G6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="H6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C7" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D7" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="E7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F7" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="G7" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="H7" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B8" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C8" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D8" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="E8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="G8" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="H8" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C9" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D9" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="E9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F9" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="G9" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="H9" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C10" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D10" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="E10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F10" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="G10" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="H10" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
   </sheetData>
@@ -13723,7 +13723,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -13731,7 +13731,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -13739,7 +13739,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -13747,7 +13747,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -13755,7 +13755,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -13763,7 +13763,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -13771,7 +13771,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -13779,7 +13779,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -13787,7 +13787,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -13795,7 +13795,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -13803,7 +13803,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -13811,7 +13811,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -13819,7 +13819,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -13827,7 +13827,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -13835,7 +13835,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -13843,7 +13843,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -13851,7 +13851,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -13859,7 +13859,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -13867,7 +13867,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -13875,7 +13875,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -13883,7 +13883,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -13891,7 +13891,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -13899,7 +13899,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -13907,7 +13907,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -13943,7 +13943,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -13951,7 +13951,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -13959,7 +13959,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -13967,7 +13967,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -13975,7 +13975,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -13983,7 +13983,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -13991,7 +13991,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -13999,7 +13999,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -14007,7 +14007,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -14015,7 +14015,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -14023,7 +14023,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -14031,7 +14031,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -14039,7 +14039,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -14047,7 +14047,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -14055,7 +14055,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -14063,7 +14063,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -14071,7 +14071,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -14079,7 +14079,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -14087,7 +14087,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -14095,7 +14095,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -14103,7 +14103,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -14111,7 +14111,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -14119,7 +14119,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -14127,7 +14127,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -14135,7 +14135,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -14143,7 +14143,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -14151,7 +14151,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -14159,7 +14159,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -14167,7 +14167,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -14175,7 +14175,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -14183,7 +14183,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -14191,7 +14191,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -14199,7 +14199,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -14207,7 +14207,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -14215,7 +14215,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -14223,7 +14223,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -14231,7 +14231,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -14239,7 +14239,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -14247,7 +14247,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -14255,7 +14255,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -14263,7 +14263,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -14271,7 +14271,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -14279,7 +14279,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B44">
         <v>43</v>
@@ -15496,7 +15496,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15504,7 +15504,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -15512,7 +15512,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15520,7 +15520,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -15528,7 +15528,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -15536,7 +15536,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -15544,7 +15544,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -15552,7 +15552,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -15560,7 +15560,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -15568,7 +15568,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -15604,7 +15604,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15612,7 +15612,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -15620,7 +15620,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15628,7 +15628,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -15636,7 +15636,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -15644,7 +15644,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -15652,7 +15652,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -15660,7 +15660,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -15668,7 +15668,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -15676,7 +15676,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -15684,7 +15684,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -15692,7 +15692,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -15700,7 +15700,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -15735,7 +15735,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15751,7 +15751,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15767,7 +15767,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -15775,7 +15775,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -15783,7 +15783,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -15791,7 +15791,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -15799,7 +15799,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -15807,7 +15807,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -15815,7 +15815,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -15823,7 +15823,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -15831,7 +15831,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -15839,7 +15839,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -15847,7 +15847,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -15878,7 +15878,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15886,7 +15886,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -15894,7 +15894,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15902,7 +15902,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -15910,7 +15910,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -15918,7 +15918,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -15926,7 +15926,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -15934,7 +15934,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -15942,7 +15942,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -15950,7 +15950,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -15958,7 +15958,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -15966,7 +15966,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -15974,7 +15974,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -15982,7 +15982,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -16018,7 +16018,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -16026,7 +16026,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -16034,7 +16034,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -16042,7 +16042,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -16050,7 +16050,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -16058,7 +16058,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -16066,7 +16066,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -16074,7 +16074,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -16082,7 +16082,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -16090,7 +16090,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -16098,7 +16098,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -16106,7 +16106,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -16114,7 +16114,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -16122,7 +16122,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -16130,7 +16130,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -16138,7 +16138,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -16146,7 +16146,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -16154,7 +16154,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -16162,7 +16162,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -16170,7 +16170,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -16178,7 +16178,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -16186,7 +16186,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -16194,7 +16194,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -16202,7 +16202,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -16210,7 +16210,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -16241,7 +16241,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -16249,7 +16249,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -16257,7 +16257,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -16348,119 +16348,119 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -16468,151 +16468,151 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B22" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B31" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -16620,298 +16620,298 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B36" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B37" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B39" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B40" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B41" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B42" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B43" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B44" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B45" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B46" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B47" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B49" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B50" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B51" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B52" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B53" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B54" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B55" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B56" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B57" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B58" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B59" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B60" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B61" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B62" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B63" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B64" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B65" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B66" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B67" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B68" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B69" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B70" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B71" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>520</v>
+      </c>
+      <c r="B72" t="s">
         <v>521</v>
-      </c>
-      <c r="B72" t="s">
-        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -16948,7 +16948,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -16956,7 +16956,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -16964,7 +16964,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -16972,7 +16972,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -16980,7 +16980,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -16988,7 +16988,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -16996,7 +16996,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -17004,7 +17004,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -17012,7 +17012,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -17020,7 +17020,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -17028,7 +17028,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -17036,7 +17036,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -17044,7 +17044,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -17052,7 +17052,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -17219,7 +17219,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -17307,7 +17307,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -17315,7 +17315,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -17323,7 +17323,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -17379,7 +17379,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -17387,7 +17387,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -17395,7 +17395,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -17403,7 +17403,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -17411,7 +17411,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -17419,7 +17419,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -17427,7 +17427,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -17435,7 +17435,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -17443,7 +17443,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -17451,7 +17451,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -17486,7 +17486,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -17494,7 +17494,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -17502,7 +17502,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -17510,7 +17510,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -17518,7 +17518,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -17526,7 +17526,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -17534,7 +17534,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -17542,7 +17542,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -17550,7 +17550,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -17558,7 +17558,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -17566,7 +17566,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -17574,7 +17574,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -17582,7 +17582,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -17590,7 +17590,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -17598,7 +17598,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -17606,7 +17606,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -17614,7 +17614,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -17622,7 +17622,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -17630,7 +17630,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -17638,7 +17638,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -17646,7 +17646,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -17654,7 +17654,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -17662,7 +17662,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -17670,7 +17670,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -17678,7 +17678,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -17686,7 +17686,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -17694,7 +17694,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -17702,7 +17702,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -17710,7 +17710,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -17718,7 +17718,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -17726,7 +17726,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -17734,7 +17734,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -17742,7 +17742,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -17750,7 +17750,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -17758,7 +17758,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -17766,7 +17766,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -17774,7 +17774,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -17782,7 +17782,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -17790,7 +17790,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -17798,7 +17798,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -17806,7 +17806,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -17814,7 +17814,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -17822,7 +17822,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B44">
         <v>43</v>
@@ -17830,7 +17830,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B45">
         <v>44</v>
@@ -17838,7 +17838,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -17872,7 +17872,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -17880,7 +17880,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -17888,7 +17888,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -17896,7 +17896,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -17904,7 +17904,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B6">
         <v>5</v>

</xml_diff>

<commit_message>
Fix to OPEX and result printing scripts
Previous version did not include O&M of VRE capacity for the off-grid electrolytic options.

Corrections to run_file that produces graphs and the one that produces CSVs outputs for editors.
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -8088,7 +8088,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Use csv for classification_titles
This should reduce the number of merge conflicts and allow us to work easier on multiple improvements in parallel.

I've kept in the files for now on how to convert it, so that we can apply this to other branches.
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="6_{A4F47DB5-C845-42B4-AA09-B0BE68E5142B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BFB3B44-282B-4E59-A59D-1D4564076705}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="6_{A4F47DB5-C845-42B4-AA09-B0BE68E5142B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53404F45-E592-43D5-96B6-64C98F36193F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -5096,7 +5096,7 @@
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -7473,8 +7473,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Connected FTT:H2 and FTT:NH3trade
Information flows between the modules
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cambridgeeconometrics-my.sharepoint.com/personal/pv_camecon_com/Documents/Documents/GitHub/FTT_H2_dev_v2/Utilities/titles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cambridgeeconometrics-my.sharepoint.com/personal/pv_camecon_com/Documents/Documents/GitHub/NH3_trade/Utilities/titles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{5CED7FD4-CBE8-4FF4-A1F6-D31781E59327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55F4631A-06B2-4063-A72D-01FFB3461402}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{5CED7FD4-CBE8-4FF4-A1F6-D31781E59327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8321F26E-36E8-418B-9099-4491D7FAAF14}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="14" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="14" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -1898,12 +1898,6 @@
     <t>grey</t>
   </si>
   <si>
-    <t>Green fertiliser</t>
-  </si>
-  <si>
-    <t>Grey fertiliser</t>
-  </si>
-  <si>
     <t>1 SMR</t>
   </si>
   <si>
@@ -2373,6 +2367,12 @@
   </si>
   <si>
     <t>Additional OPEX, mean, €/kg H2 prod.</t>
+  </si>
+  <si>
+    <t>Green market</t>
+  </si>
+  <si>
+    <t>Grey market</t>
   </si>
 </sst>
 </file>
@@ -6116,21 +6116,21 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>757</v>
+      </c>
+      <c r="B11" t="s">
+        <v>758</v>
+      </c>
+      <c r="C11" t="s">
         <v>759</v>
-      </c>
-      <c r="B11" t="s">
-        <v>760</v>
-      </c>
-      <c r="C11" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B12" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
   </sheetData>
@@ -7992,7 +7992,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -8000,7 +8000,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -8008,7 +8008,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -8016,7 +8016,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -8024,7 +8024,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -8032,7 +8032,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -8040,7 +8040,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -8048,7 +8048,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -8056,7 +8056,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -8064,7 +8064,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -8072,7 +8072,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -8087,7 +8087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78453AF4-E661-4F8D-9545-825FD7B44CDA}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -8106,7 +8106,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -8114,7 +8114,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -8122,7 +8122,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -8130,7 +8130,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -8138,7 +8138,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -8146,7 +8146,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -8154,7 +8154,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -8162,7 +8162,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -8170,7 +8170,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -8178,7 +8178,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -8186,7 +8186,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -8194,7 +8194,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -8202,7 +8202,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -8210,7 +8210,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -8218,7 +8218,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -8226,7 +8226,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -8234,7 +8234,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -8242,7 +8242,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -8250,7 +8250,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -8258,7 +8258,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -8266,7 +8266,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -8274,7 +8274,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -8282,7 +8282,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -8290,7 +8290,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -8298,7 +8298,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -8306,7 +8306,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -8340,7 +8340,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -8348,7 +8348,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -8356,7 +8356,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -8364,7 +8364,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -8607,8 +8607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A586961F-9812-40E7-9CDD-170A409422F1}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8623,7 +8623,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>610</v>
+        <v>767</v>
       </c>
       <c r="B2" t="s">
         <v>608</v>
@@ -8631,7 +8631,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>611</v>
+        <v>768</v>
       </c>
       <c r="B3" t="s">
         <v>609</v>
@@ -8662,7 +8662,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -8670,7 +8670,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -8678,7 +8678,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -8686,7 +8686,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -8694,7 +8694,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -8702,7 +8702,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -8710,7 +8710,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -8718,7 +8718,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -8726,7 +8726,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -8734,7 +8734,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -8768,7 +8768,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -8776,7 +8776,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -8784,7 +8784,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -8792,7 +8792,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -8800,7 +8800,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -8808,7 +8808,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -8816,7 +8816,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -8824,7 +8824,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -8832,7 +8832,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -8840,7 +8840,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -8848,7 +8848,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -8856,7 +8856,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B13">
         <v>11</v>
@@ -8864,7 +8864,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B14">
         <v>12</v>
@@ -8872,7 +8872,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B15">
         <v>13</v>
@@ -8880,7 +8880,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B16">
         <v>14</v>
@@ -8888,7 +8888,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B17">
         <v>15</v>
@@ -8896,7 +8896,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B18">
         <v>16</v>
@@ -8904,7 +8904,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B19">
         <v>17</v>
@@ -8912,7 +8912,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B20">
         <v>18</v>
@@ -8920,7 +8920,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B21">
         <v>19</v>
@@ -8928,7 +8928,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B22">
         <v>20</v>
@@ -8936,7 +8936,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B23">
         <v>21</v>
@@ -8944,7 +8944,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B24">
         <v>22</v>
@@ -8952,7 +8952,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B25">
         <v>23</v>
@@ -8960,7 +8960,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B26">
         <v>24</v>
@@ -8968,7 +8968,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B27">
         <v>25</v>
@@ -8976,7 +8976,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B28">
         <v>26</v>
@@ -8984,7 +8984,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B29">
         <v>27</v>
@@ -8992,7 +8992,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B30">
         <v>28</v>
@@ -9000,7 +9000,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B31">
         <v>29</v>
@@ -9008,7 +9008,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B32">
         <v>30</v>
@@ -9016,7 +9016,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B33">
         <v>31</v>
@@ -9024,7 +9024,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B34">
         <v>32</v>
@@ -9032,7 +9032,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B35">
         <v>33</v>
@@ -9040,7 +9040,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B36">
         <v>34</v>
@@ -9048,7 +9048,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B37">
         <v>35</v>
@@ -9056,7 +9056,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B38">
         <v>36</v>
@@ -9064,7 +9064,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B39">
         <v>37</v>
@@ -9072,7 +9072,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B40">
         <v>38</v>
@@ -9080,7 +9080,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B41">
         <v>39</v>
@@ -9088,7 +9088,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B42">
         <v>40</v>
@@ -9096,7 +9096,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B43">
         <v>41</v>
@@ -9104,7 +9104,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B44">
         <v>42</v>
@@ -9112,7 +9112,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B45">
         <v>43</v>
@@ -9120,7 +9120,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B46">
         <v>44</v>
@@ -9128,7 +9128,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B47">
         <v>45</v>
@@ -9136,7 +9136,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B48">
         <v>46</v>
@@ -9144,7 +9144,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B49">
         <v>47</v>
@@ -9152,7 +9152,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B50">
         <v>48</v>
@@ -9160,7 +9160,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B51">
         <v>49</v>
@@ -9168,7 +9168,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B52">
         <v>50</v>
@@ -9176,7 +9176,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B53">
         <v>51</v>
@@ -9184,7 +9184,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B54">
         <v>52</v>
@@ -9192,7 +9192,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B55">
         <v>53</v>
@@ -9200,7 +9200,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B56">
         <v>54</v>
@@ -9208,7 +9208,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B57">
         <v>55</v>
@@ -9216,7 +9216,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B58">
         <v>56</v>
@@ -9224,7 +9224,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B59">
         <v>57</v>
@@ -9232,7 +9232,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B60">
         <v>58</v>
@@ -9240,7 +9240,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B61">
         <v>59</v>
@@ -9248,7 +9248,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B62">
         <v>60</v>
@@ -9256,7 +9256,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B63">
         <v>61</v>
@@ -9264,7 +9264,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B64">
         <v>62</v>
@@ -9272,7 +9272,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B65">
         <v>63</v>
@@ -9280,7 +9280,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B66">
         <v>64</v>
@@ -9288,7 +9288,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B67">
         <v>65</v>
@@ -9296,7 +9296,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B68">
         <v>66</v>
@@ -9304,7 +9304,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B69">
         <v>67</v>
@@ -9312,7 +9312,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B70">
         <v>68</v>
@@ -9320,7 +9320,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B71">
         <v>69</v>
@@ -9328,7 +9328,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B72">
         <v>70</v>
@@ -9336,7 +9336,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B73">
         <v>71</v>
@@ -9344,7 +9344,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B74">
         <v>72</v>
@@ -9352,7 +9352,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="B75">
         <v>73</v>
@@ -9360,7 +9360,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B76">
         <v>74</v>
@@ -9368,7 +9368,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B77">
         <v>75</v>
@@ -9376,7 +9376,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B78">
         <v>76</v>
@@ -9384,7 +9384,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B79">
         <v>77</v>
@@ -9392,7 +9392,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B80">
         <v>78</v>
@@ -9400,7 +9400,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B81">
         <v>79</v>
@@ -9408,7 +9408,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B82">
         <v>80</v>
@@ -9416,7 +9416,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B83">
         <v>81</v>
@@ -9424,7 +9424,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B84">
         <v>82</v>
@@ -9432,7 +9432,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B85">
         <v>83</v>
@@ -9440,7 +9440,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B86">
         <v>84</v>
@@ -9448,7 +9448,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B87">
         <v>85</v>
@@ -9456,7 +9456,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B88">
         <v>86</v>
@@ -9464,7 +9464,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B89">
         <v>87</v>
@@ -9472,7 +9472,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B90">
         <v>88</v>
@@ -9480,7 +9480,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B91">
         <v>89</v>
@@ -9488,7 +9488,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B92">
         <v>90</v>
@@ -9496,7 +9496,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B93">
         <v>91</v>
@@ -9504,7 +9504,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B94">
         <v>92</v>
@@ -9512,7 +9512,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B95">
         <v>93</v>
@@ -9520,7 +9520,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B96">
         <v>94</v>
@@ -9528,7 +9528,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B97">
         <v>95</v>
@@ -9536,7 +9536,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B98">
         <v>96</v>
@@ -9544,7 +9544,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B99">
         <v>97</v>
@@ -9552,7 +9552,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B100">
         <v>98</v>
@@ -9560,7 +9560,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B101">
         <v>99</v>
@@ -10157,7 +10157,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B72" t="s">
         <v>570</v>

</xml_diff>

<commit_message>
Add cannibal variable to both
Not sure this is necessary, should be using just csv
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ib400\Github\FTT_StandAlone\Utilities\titles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763FFB14-A40C-4BAB-B06E-EF2B12630C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96297063-F2AB-4526-ACB9-289BED6EE753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="330" windowWidth="13480" windowHeight="10470" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="610">
   <si>
     <t>Full name</t>
   </si>
@@ -1886,6 +1886,9 @@
   </si>
   <si>
     <t>23 Value factor</t>
+  </si>
+  <si>
+    <t>24 Cannibalisation factor</t>
   </si>
 </sst>
 </file>
@@ -1895,7 +1898,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -2569,10 +2572,10 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="17"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="17"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="17"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="34" borderId="18"/>
-    <xf numFmtId="170" fontId="21" fillId="34" borderId="20"/>
+    <xf numFmtId="166" fontId="21" fillId="34" borderId="20"/>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="19"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
@@ -4562,10 +4565,10 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C01FE79-1B64-410C-BFB3-7EE7C4F3E8BE}">
   <sheetPr codeName="Sheet13"/>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -4763,6 +4766,14 @@
       </c>
       <c r="B24">
         <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>609</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merge with cascading tipping points
Main and cascading tipping points branched merged locally by Amir. This commit brings changes online.

Checked that:
- individual models run
- different combinations of power, tr, fr, and heat run
- electricity price from ftt-p can impact levelised costs in other models
</commit_message>
<xml_diff>
--- a/Utilities/titles/classification_titles.xlsx
+++ b/Utilities/titles/classification_titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Utilities/titles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\FTT_StandAlone\Utilities\titles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="6_{A4F47DB5-C845-42B4-AA09-B0BE68E5142B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53404F45-E592-43D5-96B6-64C98F36193F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E4FDA7-B28E-4631-8657-37D373620A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3375" yWindow="3375" windowWidth="21600" windowHeight="11175" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="635">
   <si>
     <t>Full name</t>
   </si>
@@ -1522,66 +1522,6 @@
     <t>10 World inflation</t>
   </si>
   <si>
-    <t>Petrol adv small</t>
-  </si>
-  <si>
-    <t>Petrol adv large</t>
-  </si>
-  <si>
-    <t>Diesel adv small</t>
-  </si>
-  <si>
-    <t>Diesel adv large</t>
-  </si>
-  <si>
-    <t>Hydrogen small</t>
-  </si>
-  <si>
-    <t>Hydrogen large</t>
-  </si>
-  <si>
-    <t>Biodiesel Large</t>
-  </si>
-  <si>
-    <t>Biodiesel Small</t>
-  </si>
-  <si>
-    <t>Bioethano Large</t>
-  </si>
-  <si>
-    <t>Bioethano Small</t>
-  </si>
-  <si>
-    <t>Electricity Large</t>
-  </si>
-  <si>
-    <t>Electricity Small</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hybrid Large </t>
-  </si>
-  <si>
-    <t>Hybrid Small</t>
-  </si>
-  <si>
-    <t>CNG/LPG Large</t>
-  </si>
-  <si>
-    <t>CNG/LPG Small</t>
-  </si>
-  <si>
-    <t>Diesel Large</t>
-  </si>
-  <si>
-    <t>Diesel Small</t>
-  </si>
-  <si>
-    <t>Petrol Large</t>
-  </si>
-  <si>
-    <t>Petrol Small</t>
-  </si>
-  <si>
     <t>1 Price of vehicles (USD/vehicle)</t>
   </si>
   <si>
@@ -1889,6 +1829,141 @@
   </si>
   <si>
     <t>21 Techs under mandate</t>
+  </si>
+  <si>
+    <t>Petrol TWV</t>
+  </si>
+  <si>
+    <t>Petrol LCV</t>
+  </si>
+  <si>
+    <t>Petrol MDT</t>
+  </si>
+  <si>
+    <t>Petrol HDT</t>
+  </si>
+  <si>
+    <t>Petrol Bus</t>
+  </si>
+  <si>
+    <t>Adv petrol TWV</t>
+  </si>
+  <si>
+    <t>Adv petrol LCV</t>
+  </si>
+  <si>
+    <t>Adv petrol MDT</t>
+  </si>
+  <si>
+    <t>Adv petrol HDT</t>
+  </si>
+  <si>
+    <t>Adv petrol Bus</t>
+  </si>
+  <si>
+    <t>Diesel TWV</t>
+  </si>
+  <si>
+    <t>Diesel LCV</t>
+  </si>
+  <si>
+    <t>Diesel MDT</t>
+  </si>
+  <si>
+    <t>Diesel HDT</t>
+  </si>
+  <si>
+    <t>Diesel Bus</t>
+  </si>
+  <si>
+    <t>Adv diesel TWV</t>
+  </si>
+  <si>
+    <t>Adv diesel LCV</t>
+  </si>
+  <si>
+    <t>Adv diesel MDT</t>
+  </si>
+  <si>
+    <t>Adv diesel HDT</t>
+  </si>
+  <si>
+    <t>Adv diesel Bus</t>
+  </si>
+  <si>
+    <t>CNG/LPG TWV</t>
+  </si>
+  <si>
+    <t>CNG/LPG LCV</t>
+  </si>
+  <si>
+    <t>CNG/LPG MDT</t>
+  </si>
+  <si>
+    <t>CNG/LPG HDT</t>
+  </si>
+  <si>
+    <t>CNG/LPG Bus</t>
+  </si>
+  <si>
+    <t>PHEV TWV</t>
+  </si>
+  <si>
+    <t>PHEV LCV</t>
+  </si>
+  <si>
+    <t>PHEV MDT</t>
+  </si>
+  <si>
+    <t>PHEV HDT</t>
+  </si>
+  <si>
+    <t>PHEV Bus</t>
+  </si>
+  <si>
+    <t>BEV TWV</t>
+  </si>
+  <si>
+    <t>BEV LCV</t>
+  </si>
+  <si>
+    <t>BEV MDT</t>
+  </si>
+  <si>
+    <t>BEV HDT</t>
+  </si>
+  <si>
+    <t>BEV Bus</t>
+  </si>
+  <si>
+    <t>Bioethanol TWV</t>
+  </si>
+  <si>
+    <t>Bioethanol LCV</t>
+  </si>
+  <si>
+    <t>Bioethanol MDT</t>
+  </si>
+  <si>
+    <t>Bioethanol HDT</t>
+  </si>
+  <si>
+    <t>Bioethanol Bus</t>
+  </si>
+  <si>
+    <t>FCEV TWV</t>
+  </si>
+  <si>
+    <t>FCEV LCV</t>
+  </si>
+  <si>
+    <t>FCEV MDT</t>
+  </si>
+  <si>
+    <t>FCEV HDT</t>
+  </si>
+  <si>
+    <t>FCEV Bus</t>
   </si>
 </sst>
 </file>
@@ -4170,7 +4245,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>591</v>
+        <v>571</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -4202,7 +4277,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>576</v>
+        <v>556</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -4210,7 +4285,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>575</v>
+        <v>555</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -4218,7 +4293,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>574</v>
+        <v>554</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -4226,7 +4301,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>573</v>
+        <v>553</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -4234,7 +4309,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -4649,7 +4724,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>606</v>
+        <v>586</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -4684,7 +4759,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>507</v>
+        <v>487</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4692,7 +4767,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>508</v>
+        <v>488</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -4708,7 +4783,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -4724,7 +4799,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>518</v>
+        <v>498</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -4740,7 +4815,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>517</v>
+        <v>497</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -4748,7 +4823,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>516</v>
+        <v>496</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -4756,7 +4831,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>515</v>
+        <v>495</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -4764,7 +4839,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>514</v>
+        <v>494</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -4772,7 +4847,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>513</v>
+        <v>493</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -4780,7 +4855,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>603</v>
+        <v>583</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -4788,7 +4863,7 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>512</v>
+        <v>492</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -4796,7 +4871,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>511</v>
+        <v>491</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -4804,7 +4879,7 @@
     </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>571</v>
+        <v>551</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -4812,7 +4887,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>510</v>
+        <v>490</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -4820,7 +4895,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -4828,7 +4903,7 @@
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>520</v>
+        <v>500</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -4836,7 +4911,7 @@
     </row>
     <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>519</v>
+        <v>499</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -4868,7 +4943,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>521</v>
+        <v>501</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4876,7 +4951,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>522</v>
+        <v>502</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5116,7 +5191,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>607</v>
+        <v>587</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5124,7 +5199,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>592</v>
+        <v>572</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5132,7 +5207,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>593</v>
+        <v>573</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -5140,7 +5215,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>594</v>
+        <v>574</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -5156,7 +5231,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>608</v>
+        <v>588</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -5164,7 +5239,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>595</v>
+        <v>575</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -5188,7 +5263,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>596</v>
+        <v>576</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -5228,7 +5303,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>597</v>
+        <v>577</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -5236,7 +5311,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>598</v>
+        <v>578</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -5244,7 +5319,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>599</v>
+        <v>579</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -5252,7 +5327,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>600</v>
+        <v>580</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -5260,7 +5335,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>601</v>
+        <v>581</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -5268,7 +5343,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>602</v>
+        <v>582</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -5276,7 +5351,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>609</v>
+        <v>589</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -5530,106 +5605,106 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>546</v>
+        <v>526</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>540</v>
+        <v>520</v>
       </c>
       <c r="B2" t="s">
-        <v>543</v>
+        <v>523</v>
       </c>
       <c r="C2" t="s">
-        <v>547</v>
+        <v>527</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>542</v>
+        <v>522</v>
       </c>
       <c r="B3" t="s">
-        <v>544</v>
+        <v>524</v>
       </c>
       <c r="C3" t="s">
-        <v>548</v>
+        <v>528</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>560</v>
+        <v>540</v>
       </c>
       <c r="B4" t="s">
-        <v>562</v>
+        <v>542</v>
       </c>
       <c r="C4" t="s">
-        <v>561</v>
+        <v>541</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>563</v>
+        <v>543</v>
       </c>
       <c r="B5" t="s">
-        <v>564</v>
+        <v>544</v>
       </c>
       <c r="C5" t="s">
-        <v>565</v>
+        <v>545</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>541</v>
+        <v>521</v>
       </c>
       <c r="B6" t="s">
-        <v>545</v>
+        <v>525</v>
       </c>
       <c r="C6" t="s">
-        <v>549</v>
+        <v>529</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>554</v>
+        <v>534</v>
       </c>
       <c r="B7" t="s">
-        <v>557</v>
+        <v>537</v>
       </c>
       <c r="C7" t="s">
-        <v>550</v>
+        <v>530</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>555</v>
+        <v>535</v>
       </c>
       <c r="B8" t="s">
-        <v>558</v>
+        <v>538</v>
       </c>
       <c r="C8" t="s">
-        <v>551</v>
+        <v>531</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>556</v>
+        <v>536</v>
       </c>
       <c r="B9" t="s">
-        <v>559</v>
+        <v>539</v>
       </c>
       <c r="C9" t="s">
-        <v>552</v>
+        <v>532</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>604</v>
+        <v>584</v>
       </c>
       <c r="B10" t="s">
-        <v>605</v>
+        <v>585</v>
       </c>
       <c r="C10" t="s">
-        <v>553</v>
+        <v>533</v>
       </c>
     </row>
   </sheetData>
@@ -7214,7 +7289,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>523</v>
+        <v>503</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7222,7 +7297,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>524</v>
+        <v>504</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -7230,7 +7305,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>525</v>
+        <v>505</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7238,7 +7313,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>526</v>
+        <v>506</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -7246,7 +7321,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>527</v>
+        <v>507</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -7254,7 +7329,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>528</v>
+        <v>508</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -7262,7 +7337,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>529</v>
+        <v>509</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -7270,7 +7345,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>530</v>
+        <v>510</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -7278,7 +7353,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>531</v>
+        <v>511</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -7286,7 +7361,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>532</v>
+        <v>512</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -7294,7 +7369,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>533</v>
+        <v>513</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -7302,7 +7377,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>534</v>
+        <v>514</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -7310,7 +7385,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>535</v>
+        <v>515</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -7345,7 +7420,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>536</v>
+        <v>516</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -7361,7 +7436,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>537</v>
+        <v>517</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7377,7 +7452,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>538</v>
+        <v>518</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -7385,7 +7460,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>539</v>
+        <v>519</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -7457,7 +7532,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>511</v>
+        <v>491</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -7473,7 +7548,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -7677,7 +7752,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>568</v>
+        <v>548</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -7685,7 +7760,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>569</v>
+        <v>549</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -8281,10 +8356,10 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>566</v>
+        <v>546</v>
       </c>
       <c r="B72" t="s">
-        <v>567</v>
+        <v>547</v>
       </c>
     </row>
   </sheetData>
@@ -8592,7 +8667,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>577</v>
+        <v>557</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -8680,7 +8755,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -8688,7 +8763,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>579</v>
+        <v>559</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -8696,7 +8771,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>580</v>
+        <v>560</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -8752,7 +8827,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>581</v>
+        <v>561</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -8760,7 +8835,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>582</v>
+        <v>562</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -8768,7 +8843,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>583</v>
+        <v>563</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -8776,7 +8851,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>584</v>
+        <v>564</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -8784,7 +8859,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>585</v>
+        <v>565</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -8792,7 +8867,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>586</v>
+        <v>566</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -8800,7 +8875,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>587</v>
+        <v>567</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -8808,7 +8883,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>588</v>
+        <v>568</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -8816,7 +8891,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>589</v>
+        <v>569</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -8824,7 +8899,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>590</v>
+        <v>570</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -8838,10 +8913,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56AA3A07-21BA-4ACD-867A-E4F0D5D67CE0}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:AW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8859,7 +8934,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>506</v>
+        <v>590</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -8867,7 +8942,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>505</v>
+        <v>591</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -8875,7 +8950,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>487</v>
+        <v>592</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -8883,7 +8958,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>488</v>
+        <v>593</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -8891,7 +8966,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>504</v>
+        <v>594</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -8899,7 +8974,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>503</v>
+        <v>595</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -8907,7 +8982,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>489</v>
+        <v>596</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -8915,7 +8990,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>490</v>
+        <v>597</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -8923,7 +8998,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>502</v>
+        <v>598</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -8931,7 +9006,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>501</v>
+        <v>599</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -8939,7 +9014,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -8947,7 +9022,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>499</v>
+        <v>601</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -8955,7 +9030,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>498</v>
+        <v>602</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -8963,7 +9038,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>497</v>
+        <v>603</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -8971,7 +9046,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>496</v>
+        <v>604</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -8979,7 +9054,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>495</v>
+        <v>605</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -8987,7 +9062,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>494</v>
+        <v>606</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -8995,7 +9070,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>493</v>
+        <v>607</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -9003,7 +9078,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>491</v>
+        <v>608</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -9011,10 +9086,210 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>492</v>
+        <v>609</v>
       </c>
       <c r="B21">
         <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>610</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>611</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>612</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>613</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>614</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>615</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>616</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>617</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>618</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>619</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>620</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>621</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>622</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>623</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>624</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>625</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>626</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>627</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>628</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>629</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>630</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>631</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>632</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>633</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>634</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>